<commit_message>
added validation data and reference model for AS3
</commit_message>
<xml_diff>
--- a/MercuryModel.xlsx
+++ b/MercuryModel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d679a80baeebce9/Documents/TU-Delft/AE4893 Physics of Planetary interiors/Assignment 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d679a80baeebce9/Documents/TU-Delft/AE4893 Physics of Planetary interiors/Assignment 3/PPI_AS3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="409" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20838096-6AD7-4900-B548-752FF82E1F0F}"/>
+  <xr:revisionPtr revIDLastSave="504" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71A0569-121E-4744-A1B5-18F9B6E22FF2}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,26 +49,26 @@
     <author>tc={7DA81649-5212-4E57-A568-C51ABC13044F}</author>
     <author>tc={2C949B62-2D82-43E1-8F44-68F37F84B118}</author>
     <author>tc={7049D5AF-F941-4404-A0B2-918327215D5D}</author>
-    <author>tc={388FB68A-BD01-437E-84E8-95E44E0FA41E}</author>
     <author>tc={BC381252-9396-479B-9D06-1C5046FBE7A0}</author>
     <author>tc={EC67E508-62B0-482E-B662-537ACDBAE5C1}</author>
     <author>tc={F278D8B4-A4E9-4A3D-9669-608573FB7CD2}</author>
     <author>tc={A3EA189A-8C2D-466A-92CF-88755F03C8E5}</author>
-    <author>tc={AF0A2A2B-B375-4007-97E0-483D8B1CF039}</author>
-    <author>tc={4BFCC566-92E8-4928-8748-52B17BD7C38D}</author>
     <author>tc={B1FFF1BF-D043-4A41-8B27-719EC45AF9FF}</author>
     <author>tc={F48003B8-D140-4E90-9B5B-4178EA282500}</author>
-    <author>tc={A4073D4E-E1DC-44B0-9181-10733F210188}</author>
     <author>tc={C3E5C6F5-5ED5-404B-97BD-E2A7C533B18A}</author>
     <author>tc={8DF685AD-704D-4C77-BEBD-0D63FCCE22B6}</author>
     <author>tc={76C5837A-6C3B-4CC7-A0A4-9F4A8BEBD2A0}</author>
     <author>tc={4076FCF4-00F1-4557-BF5C-E835DC09D8C3}</author>
+    <author>tc={388FB68A-BD01-437E-84E8-95E44E0FA41E}</author>
     <author>tc={726C3CA8-FBDE-4D90-9780-4C5C11281E37}</author>
     <author>tc={62659B77-C5F0-43BE-AE56-F1DB4C81BEC7}</author>
     <author>tc={6EAC48A1-DE7E-44BF-A400-14FFD0D6EA9F}</author>
+    <author>tc={AF0A2A2B-B375-4007-97E0-483D8B1CF039}</author>
+    <author>tc={4BFCC566-92E8-4928-8748-52B17BD7C38D}</author>
     <author>tc={3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}</author>
     <author>tc={17382DD3-3CC6-4944-922C-7ED195CF53C3}</author>
     <author>tc={4805467D-952B-41B4-86D7-6B034FCD91D7}</author>
+    <author>tc={A4073D4E-E1DC-44B0-9181-10733F210188}</author>
     <author>tc={7C0DD50C-3623-48FA-84D7-1EF1D30CD771}</author>
     <author>tc={46C7DEB7-FDA7-4ECC-B5F2-0B6956A449A2}</author>
     <author>tc={7EC2AF2B-D535-47E2-9C1D-2D569E41F041}</author>
@@ -139,15 +139,7 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="AB26" authorId="6" shapeId="0" xr:uid="{388FB68A-BD01-437E-84E8-95E44E0FA41E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Recomputed for ts=Dref from AS2</t>
-      </text>
-    </comment>
-    <comment ref="W27" authorId="7" shapeId="0" xr:uid="{BC381252-9396-479B-9D06-1C5046FBE7A0}">
+    <comment ref="W27" authorId="6" shapeId="0" xr:uid="{BC381252-9396-479B-9D06-1C5046FBE7A0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -155,7 +147,7 @@
     Free var</t>
       </text>
     </comment>
-    <comment ref="O28" authorId="8" shapeId="0" xr:uid="{EC67E508-62B0-482E-B662-537ACDBAE5C1}">
+    <comment ref="O28" authorId="7" shapeId="0" xr:uid="{EC67E508-62B0-482E-B662-537ACDBAE5C1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -163,7 +155,7 @@
     Free var</t>
       </text>
     </comment>
-    <comment ref="T28" authorId="9" shapeId="0" xr:uid="{F278D8B4-A4E9-4A3D-9669-608573FB7CD2}">
+    <comment ref="T28" authorId="8" shapeId="0" xr:uid="{F278D8B4-A4E9-4A3D-9669-608573FB7CD2}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -177,7 +169,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="U28" authorId="10" shapeId="0" xr:uid="{A3EA189A-8C2D-466A-92CF-88755F03C8E5}">
+    <comment ref="U28" authorId="9" shapeId="0" xr:uid="{A3EA189A-8C2D-466A-92CF-88755F03C8E5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -185,7 +177,7 @@
     =Dref, Te=NA</t>
       </text>
     </comment>
-    <comment ref="AB28" authorId="11" shapeId="0" xr:uid="{AF0A2A2B-B375-4007-97E0-483D8B1CF039}">
+    <comment ref="L29" authorId="10" shapeId="0" xr:uid="{B1FFF1BF-D043-4A41-8B27-719EC45AF9FF}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -199,15 +191,71 @@
 </t>
       </text>
     </comment>
-    <comment ref="AC28" authorId="12" shapeId="0" xr:uid="{4BFCC566-92E8-4928-8748-52B17BD7C38D}">
+    <comment ref="T30" authorId="11" shapeId="0" xr:uid="{F48003B8-D140-4E90-9B5B-4178EA282500}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Fe,liq
+Fe,sol
+Fe3S,sol
+FeSV,sol
+</t>
+      </text>
+    </comment>
+    <comment ref="H31" authorId="12" shapeId="0" xr:uid="{C3E5C6F5-5ED5-404B-97BD-E2A7C533B18A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    =Dref, Te=NA</t>
+    Read from xs=0.05 on Fig3</t>
       </text>
     </comment>
-    <comment ref="L29" authorId="13" shapeId="0" xr:uid="{B1FFF1BF-D043-4A41-8B27-719EC45AF9FF}">
+    <comment ref="J31" authorId="13" shapeId="0" xr:uid="{8DF685AD-704D-4C77-BEBD-0D63FCCE22B6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Read from Fig2</t>
+      </text>
+    </comment>
+    <comment ref="L31" authorId="14" shapeId="0" xr:uid="{76C5837A-6C3B-4CC7-A0A4-9F4A8BEBD2A0}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Fe,liq
+Fe,sol
+Fe3S,sol
+FeSV,sol
+</t>
+      </text>
+    </comment>
+    <comment ref="J32" authorId="15" shapeId="0" xr:uid="{4076FCF4-00F1-4557-BF5C-E835DC09D8C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Read from Fig2</t>
+      </text>
+    </comment>
+    <comment ref="AB34" authorId="16" shapeId="0" xr:uid="{388FB68A-BD01-437E-84E8-95E44E0FA41E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Recomputed for ts=Dref from AS2</t>
+      </text>
+    </comment>
+    <comment ref="W35" authorId="17" shapeId="0" xr:uid="{726C3CA8-FBDE-4D90-9780-4C5C11281E37}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Free var</t>
+      </text>
+    </comment>
+    <comment ref="T36" authorId="18" shapeId="0" xr:uid="{62659B77-C5F0-43BE-AE56-F1DB4C81BEC7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -221,75 +269,15 @@
 </t>
       </text>
     </comment>
-    <comment ref="T30" authorId="14" shapeId="0" xr:uid="{F48003B8-D140-4E90-9B5B-4178EA282500}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Fe,liq
-Fe,sol
-Fe3S,sol
-FeSV,sol
-</t>
-      </text>
-    </comment>
-    <comment ref="AB30" authorId="15" shapeId="0" xr:uid="{A4073D4E-E1DC-44B0-9181-10733F210188}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Fe,liq
-Fe,sol
-Fe3S,sol
-FeSV,sol
-</t>
-      </text>
-    </comment>
-    <comment ref="H31" authorId="16" shapeId="0" xr:uid="{C3E5C6F5-5ED5-404B-97BD-E2A7C533B18A}">
+    <comment ref="U36" authorId="19" shapeId="0" xr:uid="{6EAC48A1-DE7E-44BF-A400-14FFD0D6EA9F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Read from xs=0.05 on Fig3</t>
+    =Dref, Te=NA</t>
       </text>
     </comment>
-    <comment ref="J31" authorId="17" shapeId="0" xr:uid="{8DF685AD-704D-4C77-BEBD-0D63FCCE22B6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Read from Fig2</t>
-      </text>
-    </comment>
-    <comment ref="L31" authorId="18" shapeId="0" xr:uid="{76C5837A-6C3B-4CC7-A0A4-9F4A8BEBD2A0}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Fe,liq
-Fe,sol
-Fe3S,sol
-FeSV,sol
-</t>
-      </text>
-    </comment>
-    <comment ref="J32" authorId="19" shapeId="0" xr:uid="{4076FCF4-00F1-4557-BF5C-E835DC09D8C3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Read from Fig2</t>
-      </text>
-    </comment>
-    <comment ref="W35" authorId="20" shapeId="0" xr:uid="{726C3CA8-FBDE-4D90-9780-4C5C11281E37}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Free var</t>
-      </text>
-    </comment>
-    <comment ref="T36" authorId="21" shapeId="0" xr:uid="{62659B77-C5F0-43BE-AE56-F1DB4C81BEC7}">
+    <comment ref="AB36" authorId="20" shapeId="0" xr:uid="{AF0A2A2B-B375-4007-97E0-483D8B1CF039}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -303,7 +291,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="U36" authorId="22" shapeId="0" xr:uid="{6EAC48A1-DE7E-44BF-A400-14FFD0D6EA9F}">
+    <comment ref="AC36" authorId="21" shapeId="0" xr:uid="{4BFCC566-92E8-4928-8748-52B17BD7C38D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -311,7 +299,7 @@
     =Dref, Te=NA</t>
       </text>
     </comment>
-    <comment ref="H38" authorId="23" shapeId="0" xr:uid="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
+    <comment ref="H38" authorId="22" shapeId="0" xr:uid="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -319,7 +307,7 @@
     Read from xs=0.05 on Fig3</t>
       </text>
     </comment>
-    <comment ref="J38" authorId="24" shapeId="0" xr:uid="{17382DD3-3CC6-4944-922C-7ED195CF53C3}">
+    <comment ref="J38" authorId="23" shapeId="0" xr:uid="{17382DD3-3CC6-4944-922C-7ED195CF53C3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +315,19 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="T38" authorId="25" shapeId="0" xr:uid="{4805467D-952B-41B4-86D7-6B034FCD91D7}">
+    <comment ref="T38" authorId="24" shapeId="0" xr:uid="{4805467D-952B-41B4-86D7-6B034FCD91D7}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Fe,liq
+Fe,sol
+Fe3S,sol
+FeSV,sol
+</t>
+      </text>
+    </comment>
+    <comment ref="AB38" authorId="25" shapeId="0" xr:uid="{A4073D4E-E1DC-44B0-9181-10733F210188}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="240">
   <si>
     <t>T_0</t>
   </si>
@@ -1167,21 +1167,9 @@
     <t>v</t>
   </si>
   <si>
-    <t>k_2,u</t>
-  </si>
-  <si>
-    <t>h_2,u</t>
-  </si>
-  <si>
     <t>AS3.S1</t>
   </si>
   <si>
-    <t>AS3.S3</t>
-  </si>
-  <si>
-    <t>k2</t>
-  </si>
-  <si>
     <t>whole</t>
   </si>
   <si>
@@ -1201,6 +1189,33 @@
   </si>
   <si>
     <t>viscosity [Pa s]</t>
+  </si>
+  <si>
+    <t>AS3.S7</t>
+  </si>
+  <si>
+    <t>Fig17, S3</t>
+  </si>
+  <si>
+    <t>Fig4,S1</t>
+  </si>
+  <si>
+    <t>value (k2)</t>
+  </si>
+  <si>
+    <t>value (h2)</t>
+  </si>
+  <si>
+    <t>S3, RCMB=1326km</t>
+  </si>
+  <si>
+    <t>S3, sweep RCMB</t>
+  </si>
+  <si>
+    <t>S1, 3-layered</t>
+  </si>
+  <si>
+    <t>S1, fluid</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1226,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,12 +1265,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1342,7 +1351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1353,38 +1362,24 @@
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000E+00"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1704,6 +1699,12 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1715,6 +1716,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>600635</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>559306</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>151924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8127941-2A01-48FA-8CA6-34B5774185A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21497364" y="2366683"/>
+          <a:ext cx="3006671" cy="1909006"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>344715</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94527923-C236-061D-BE73-1357843D843B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24837572" y="2358571"/>
+          <a:ext cx="2195286" cy="2065555"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1750,8 +1844,8 @@
     <sortCondition ref="B1:B17"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{20C5EE52-CB95-4685-969E-41D3915E735F}" uniqueName="1" name="core" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{C2537B62-B949-40E2-AAC0-A79313442393}" uniqueName="2" name="mantle" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{20C5EE52-CB95-4685-969E-41D3915E735F}" uniqueName="1" name="core" queryTableFieldId="1" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{C2537B62-B949-40E2-AAC0-A79313442393}" uniqueName="2" name="mantle" queryTableFieldId="2" dataDxfId="54"/>
     <tableColumn id="3" xr3:uid="{FE59BD27-3791-414C-85F9-F35B7FB27FF6}" uniqueName="3" name="ICB radius [km]" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{6D68B10F-46E5-4D6A-91C7-AB57C8E7A50D}" uniqueName="4" name="CMB radius [km]" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{D63DBD22-7DEB-4253-9CA4-41A3979F2571}" uniqueName="5" name="sulfur content [%]" queryTableFieldId="5"/>
@@ -1767,43 +1861,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F152EC5-3DC0-4D91-AD22-069EC150492F}" name="material" displayName="material" ref="D3:AN87" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F152EC5-3DC0-4D91-AD22-069EC150492F}" name="material" displayName="material" ref="D3:AN87" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="D3:AN87" xr:uid="{8F152EC5-3DC0-4D91-AD22-069EC150492F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:AK87">
     <sortCondition ref="D3:D87"/>
   </sortState>
   <tableColumns count="37">
-    <tableColumn id="1" xr3:uid="{C6859E7A-0DF3-4B66-A62D-FC887233952D}" name="material" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{F6E5D82F-B4A4-404F-A63B-B821D7BCB98E}" name="T_ref [K]" dataDxfId="52"/>
-    <tableColumn id="18" xr3:uid="{07B53A00-DA15-4254-8917-B80BA01C64A3}" name="p_ref [Gpa]" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{A5A8CFB9-C5D9-4852-9FED-65CEEB36C603}" name="rho_0 [kg/m3]" dataDxfId="50"/>
-    <tableColumn id="21" xr3:uid="{5731FD37-CA6D-4179-AE5B-D637F4A961ED}" name="drho/dp" dataDxfId="49"/>
-    <tableColumn id="22" xr3:uid="{D4831BAC-304E-4F35-9628-00666DB71886}" name="drho/dT" dataDxfId="48"/>
-    <tableColumn id="23" xr3:uid="{FE74C40C-67B1-41E0-B19E-8BF5DD3F7314}" name="drho/dXs" dataDxfId="47"/>
-    <tableColumn id="24" xr3:uid="{5DFF8098-7226-436B-864E-D311AC61D033}" name="drho/dXs^2" dataDxfId="46"/>
-    <tableColumn id="25" xr3:uid="{82D1B38C-1712-4F37-A3FD-B94A7A70396E}" name="rho [kg/m3]" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{C6859E7A-0DF3-4B66-A62D-FC887233952D}" name="material" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{F6E5D82F-B4A4-404F-A63B-B821D7BCB98E}" name="T_ref [K]" dataDxfId="50"/>
+    <tableColumn id="18" xr3:uid="{07B53A00-DA15-4254-8917-B80BA01C64A3}" name="p_ref [Gpa]" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{A5A8CFB9-C5D9-4852-9FED-65CEEB36C603}" name="rho_0 [kg/m3]" dataDxfId="48"/>
+    <tableColumn id="21" xr3:uid="{5731FD37-CA6D-4179-AE5B-D637F4A961ED}" name="drho/dp" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{D4831BAC-304E-4F35-9628-00666DB71886}" name="drho/dT" dataDxfId="46"/>
+    <tableColumn id="23" xr3:uid="{FE74C40C-67B1-41E0-B19E-8BF5DD3F7314}" name="drho/dXs" dataDxfId="45"/>
+    <tableColumn id="24" xr3:uid="{5DFF8098-7226-436B-864E-D311AC61D033}" name="drho/dXs^2" dataDxfId="44"/>
+    <tableColumn id="25" xr3:uid="{82D1B38C-1712-4F37-A3FD-B94A7A70396E}" name="rho [kg/m3]" dataDxfId="43">
       <calculatedColumnFormula>material[[#This Row],[rho_0 '[kg/m3']]]+material[[#This Row],[drho/dp]]*(material[[#This Row],[p]]-material[[#This Row],[p_ref '[Gpa']]])+material[[#This Row],[drho/dT]]*(material[[#This Row],[T]]-material[[#This Row],[T_ref '[K']]])+material[[#This Row],[drho/dXs]]*material[[#This Row],[sulfur fraction X_s]]+material[[#This Row],[drho/dXs^2]]*material[[#This Row],[sulfur fraction X_s]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{53EB9943-896E-4065-8FE7-E886883D9B0A}" name="K_0 [Gpa]" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{B158C837-6B72-4F18-86F1-E880C837C010}" name="dK/dT" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{34CBCE32-97CF-4DF6-9453-699F8313430A}" name="dK/dp [-]" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{38064A0F-3D48-4067-AE97-A58C75F0C794}" name="dK/dXs" dataDxfId="41"/>
-    <tableColumn id="20" xr3:uid="{B3989610-1A9A-4F4B-89F3-769E49549DB9}" name="dK/dXs^2" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{66B8EF54-0900-4856-9ABC-B5708FF2A5E9}" name="K [GPa]" dataDxfId="39"/>
-    <tableColumn id="26" xr3:uid="{0A189309-2D9F-4F55-B6E2-9B450A654D06}" name="a_0" dataDxfId="38"/>
-    <tableColumn id="28" xr3:uid="{7683C7ED-A7ED-46EB-92F9-B53D5CD047D8}" name="da/dp" dataDxfId="37"/>
-    <tableColumn id="27" xr3:uid="{39F221DB-9BC6-4843-AE53-39C4B9917F1E}" name="da/dT" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{1140898D-2BCA-4FFB-9E1A-AD4E4C640AD5}" name="a [1/K]" dataDxfId="35">
+    <tableColumn id="15" xr3:uid="{53EB9943-896E-4065-8FE7-E886883D9B0A}" name="K_0 [Gpa]" dataDxfId="42"/>
+    <tableColumn id="16" xr3:uid="{B158C837-6B72-4F18-86F1-E880C837C010}" name="dK/dT" dataDxfId="41"/>
+    <tableColumn id="17" xr3:uid="{34CBCE32-97CF-4DF6-9453-699F8313430A}" name="dK/dp [-]" dataDxfId="40"/>
+    <tableColumn id="19" xr3:uid="{38064A0F-3D48-4067-AE97-A58C75F0C794}" name="dK/dXs" dataDxfId="39"/>
+    <tableColumn id="20" xr3:uid="{B3989610-1A9A-4F4B-89F3-769E49549DB9}" name="dK/dXs^2" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{66B8EF54-0900-4856-9ABC-B5708FF2A5E9}" name="K [GPa]" dataDxfId="37"/>
+    <tableColumn id="26" xr3:uid="{0A189309-2D9F-4F55-B6E2-9B450A654D06}" name="a_0" dataDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{7683C7ED-A7ED-46EB-92F9-B53D5CD047D8}" name="da/dp" dataDxfId="35"/>
+    <tableColumn id="27" xr3:uid="{39F221DB-9BC6-4843-AE53-39C4B9917F1E}" name="da/dT" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{1140898D-2BCA-4FFB-9E1A-AD4E4C640AD5}" name="a [1/K]" dataDxfId="33">
       <calculatedColumnFormula>material[[#This Row],[a_0]]+material[[#This Row],[da/dp]]*(material[[#This Row],[p]]-material[[#This Row],[p_ref '[Gpa']]])+material[[#This Row],[da/dT]]*(material[[#This Row],[T]]-material[[#This Row],[T_ref '[K']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{932E46EA-B6F3-4F0E-9ED2-E288F02B4C18}" name="y=a*Ks/rho*Cp" dataDxfId="34"/>
-    <tableColumn id="35" xr3:uid="{B2C8CBC1-B5B0-49F2-A1FE-579BCB44E9A5}" name="Mw [g/mol]" dataDxfId="33"/>
-    <tableColumn id="30" xr3:uid="{ABC12D5A-E7AD-4FBF-B0B8-40E8EA1BF9BB}" name="Cp_A" dataDxfId="32"/>
-    <tableColumn id="31" xr3:uid="{C6FCB0FF-5B08-47FC-B357-C60260E2565D}" name="Cp_B" dataDxfId="31"/>
-    <tableColumn id="32" xr3:uid="{CA4903F7-4184-4091-A6B9-41D53288A3CF}" name="Cp_C" dataDxfId="30"/>
-    <tableColumn id="33" xr3:uid="{636A47CB-5086-4F02-9592-E4E48C59FCA8}" name="Cp_D" dataDxfId="29"/>
-    <tableColumn id="34" xr3:uid="{D08328F9-D071-44F0-B944-BFDD25591F48}" name="Cp_E" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{4B7E1A24-18E1-4382-A5EB-1651FF63E55E}" name="Cp [J/Kkg]" dataDxfId="27">
+    <tableColumn id="8" xr3:uid="{932E46EA-B6F3-4F0E-9ED2-E288F02B4C18}" name="y=a*Ks/rho*Cp" dataDxfId="32"/>
+    <tableColumn id="35" xr3:uid="{B2C8CBC1-B5B0-49F2-A1FE-579BCB44E9A5}" name="Mw [g/mol]" dataDxfId="31"/>
+    <tableColumn id="30" xr3:uid="{ABC12D5A-E7AD-4FBF-B0B8-40E8EA1BF9BB}" name="Cp_A" dataDxfId="30"/>
+    <tableColumn id="31" xr3:uid="{C6FCB0FF-5B08-47FC-B357-C60260E2565D}" name="Cp_B" dataDxfId="29"/>
+    <tableColumn id="32" xr3:uid="{CA4903F7-4184-4091-A6B9-41D53288A3CF}" name="Cp_C" dataDxfId="28"/>
+    <tableColumn id="33" xr3:uid="{636A47CB-5086-4F02-9592-E4E48C59FCA8}" name="Cp_D" dataDxfId="27"/>
+    <tableColumn id="34" xr3:uid="{D08328F9-D071-44F0-B944-BFDD25591F48}" name="Cp_E" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{4B7E1A24-18E1-4382-A5EB-1651FF63E55E}" name="Cp [J/Kkg]" dataDxfId="25">
       <calculatedColumnFormula>IFERROR(IFERROR(
 (material[[#This Row],[Cp_A]]+material[[#This Row],[Cp_B]]*material[[#This Row],[T]]+material[[#This Row],[Cp_C]]*material[[#This Row],[T]]^2+material[[#This Row],[Cp_D]]*material[[#This Row],[T]]^3+IF(material[[#This Row],[T]]=0,0,material[[#This Row],[Cp_E]]*material[[#This Row],[T]]^(-2)))*1000/material[[#This Row],[Mw '[g/mol']]],
 IF(material[[#This Row],[Cp_A]]=0,
@@ -1811,38 +1905,38 @@
 material[[#This Row],[Cp_A]])),
 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{D38386FE-69C3-48E8-B0A5-ED94BD59C49A}" name="ⲕ [Wm2/J]" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{D3751735-7FA4-4EF8-BF83-E9D9E98C816E}" name="k [W/mK]" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{7F80310E-B14F-43E9-BE34-C2DE641131BB}" name="visc [mPas]" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{D05CB256-DD72-4247-A7CE-9EA7AAA8C0D0}" name="sulfur fraction X_s" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{E8E3F2F8-72BA-49CA-9EF4-2963CE5210B6}" name="T" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{B1C79DCC-06F7-4B0A-B79D-54CBE24629A0}" name="p" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{701B42F1-1012-4484-837E-90A70B6C87AF}" name="source main" dataDxfId="20"/>
-    <tableColumn id="36" xr3:uid="{085C3B51-EF7F-4D7A-A135-47EBE7D58B18}" name="source k" dataDxfId="19"/>
-    <tableColumn id="37" xr3:uid="{FB2C063D-6C00-4EF2-9669-7959CD4C0914}" name="source Cp" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{36E21241-244F-4662-B150-CB74F3043303}" name="Column1" dataDxfId="17"/>
+    <tableColumn id="29" xr3:uid="{D38386FE-69C3-48E8-B0A5-ED94BD59C49A}" name="ⲕ [Wm2/J]" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{D3751735-7FA4-4EF8-BF83-E9D9E98C816E}" name="k [W/mK]" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{7F80310E-B14F-43E9-BE34-C2DE641131BB}" name="visc [mPas]" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{D05CB256-DD72-4247-A7CE-9EA7AAA8C0D0}" name="sulfur fraction X_s" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{E8E3F2F8-72BA-49CA-9EF4-2963CE5210B6}" name="T" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{B1C79DCC-06F7-4B0A-B79D-54CBE24629A0}" name="p" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{701B42F1-1012-4484-837E-90A70B6C87AF}" name="source main" dataDxfId="18"/>
+    <tableColumn id="36" xr3:uid="{085C3B51-EF7F-4D7A-A135-47EBE7D58B18}" name="source k" dataDxfId="17"/>
+    <tableColumn id="37" xr3:uid="{FB2C063D-6C00-4EF2-9669-7959CD4C0914}" name="source Cp" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{36E21241-244F-4662-B150-CB74F3043303}" name="Column1" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4815E85E-8978-4E58-A8B4-C54F1A6E8AFC}" name="MatExport" displayName="MatExport" ref="AW37:BI47" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4815E85E-8978-4E58-A8B4-C54F1A6E8AFC}" name="MatExport" displayName="MatExport" ref="AW37:BI47" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="AW37:BI47" xr:uid="{4815E85E-8978-4E58-A8B4-C54F1A6E8AFC}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F6FE93EA-3012-453E-9F91-0F4FB76E176D}" name="material" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{14A69B19-D486-4EB2-A643-02FAF87BCD81}" name="T_ref" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{AA4FE1FC-8212-48FF-9A1C-986A51437120}" name="p_ref" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{2ADE5AEE-29E6-4A2D-ABFA-55ECB48F5B87}" name="rho_0" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{FC1E0FB6-4A3E-4740-B9BC-889E6C7A9E65}" name="drho/dXs" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{A7C008F8-EEED-40A5-831A-C365734042C3}" name="drho/dXs2" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{B3C3650C-BFEB-4E5D-A746-E3CFEC768C51}" name="K_0" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{0EB6F5A1-2F4A-4603-8982-416BF2CE2B43}" name="dK/dXs" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{369685E0-D572-44B0-9273-FBB14C070FC9}" name="dK/dXs2" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{7BC71007-165C-4124-9A5D-380FCBE6E15B}" name="a_0" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D42EBF64-9248-4A14-A086-DA9361F19AB1}" name="Cp" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{58627E0E-356C-48DB-827E-B72884FD60D2}" name="k" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{3BE9AE2E-6400-4848-A028-E66BADFC8516}" name="visc" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F6FE93EA-3012-453E-9F91-0F4FB76E176D}" name="material" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{14A69B19-D486-4EB2-A643-02FAF87BCD81}" name="T_ref" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{AA4FE1FC-8212-48FF-9A1C-986A51437120}" name="p_ref" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{2ADE5AEE-29E6-4A2D-ABFA-55ECB48F5B87}" name="rho_0" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{FC1E0FB6-4A3E-4740-B9BC-889E6C7A9E65}" name="drho/dXs" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{A7C008F8-EEED-40A5-831A-C365734042C3}" name="drho/dXs2" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{B3C3650C-BFEB-4E5D-A746-E3CFEC768C51}" name="K_0" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{0EB6F5A1-2F4A-4603-8982-416BF2CE2B43}" name="dK/dXs" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{369685E0-D572-44B0-9273-FBB14C070FC9}" name="dK/dXs2" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{7BC71007-165C-4124-9A5D-380FCBE6E15B}" name="a_0" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{D42EBF64-9248-4A14-A086-DA9361F19AB1}" name="Cp" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{58627E0E-356C-48DB-827E-B72884FD60D2}" name="k" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3BE9AE2E-6400-4848-A028-E66BADFC8516}" name="visc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2139,9 +2233,6 @@
   <threadedComment ref="J24" dT="2024-04-30T15:24:13.23" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{7049D5AF-F941-4404-A0B2-918327215D5D}">
     <text>Read from Fig2</text>
   </threadedComment>
-  <threadedComment ref="AB26" dT="2024-06-27T12:50:10.12" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{388FB68A-BD01-437E-84E8-95E44E0FA41E}">
-    <text>Recomputed for ts=Dref from AS2</text>
-  </threadedComment>
   <threadedComment ref="W27" dT="2024-06-05T14:52:30.26" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{BC381252-9396-479B-9D06-1C5046FBE7A0}">
     <text>Free var</text>
   </threadedComment>
@@ -2160,18 +2251,6 @@
   <threadedComment ref="U28" dT="2024-06-27T12:12:15.58" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{A3EA189A-8C2D-466A-92CF-88755F03C8E5}">
     <text>=Dref, Te=NA</text>
   </threadedComment>
-  <threadedComment ref="AB28" dT="2024-06-05T14:59:07.25" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{AF0A2A2B-B375-4007-97E0-483D8B1CF039}">
-    <text xml:space="preserve">MA
-FC
-FC
-FC
-MA
-crust
-</text>
-  </threadedComment>
-  <threadedComment ref="AC28" dT="2024-06-27T12:12:15.58" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{4BFCC566-92E8-4928-8748-52B17BD7C38D}">
-    <text>=Dref, Te=NA</text>
-  </threadedComment>
   <threadedComment ref="L29" dT="2024-06-05T14:59:07.25" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{B1FFF1BF-D043-4A41-8B27-719EC45AF9FF}">
     <text xml:space="preserve">MA
 FC
@@ -2182,13 +2261,6 @@
 </text>
   </threadedComment>
   <threadedComment ref="T30" dT="2024-06-05T14:59:36.31" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{F48003B8-D140-4E90-9B5B-4178EA282500}">
-    <text xml:space="preserve">Fe,liq
-Fe,sol
-Fe3S,sol
-FeSV,sol
-</text>
-  </threadedComment>
-  <threadedComment ref="AB30" dT="2024-06-05T14:59:36.31" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{A4073D4E-E1DC-44B0-9181-10733F210188}">
     <text xml:space="preserve">Fe,liq
 Fe,sol
 Fe3S,sol
@@ -2211,6 +2283,9 @@
   <threadedComment ref="J32" dT="2024-04-30T15:24:13.23" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{4076FCF4-00F1-4557-BF5C-E835DC09D8C3}">
     <text>Read from Fig2</text>
   </threadedComment>
+  <threadedComment ref="AB34" dT="2024-06-27T12:50:10.12" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{388FB68A-BD01-437E-84E8-95E44E0FA41E}">
+    <text>Recomputed for ts=Dref from AS2</text>
+  </threadedComment>
   <threadedComment ref="W35" dT="2024-06-05T14:52:30.26" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{726C3CA8-FBDE-4D90-9780-4C5C11281E37}">
     <text>Free var</text>
   </threadedComment>
@@ -2226,6 +2301,18 @@
   <threadedComment ref="U36" dT="2024-06-27T12:12:15.58" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{6EAC48A1-DE7E-44BF-A400-14FFD0D6EA9F}">
     <text>=Dref, Te=NA</text>
   </threadedComment>
+  <threadedComment ref="AB36" dT="2024-06-05T14:59:07.25" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{AF0A2A2B-B375-4007-97E0-483D8B1CF039}">
+    <text xml:space="preserve">MA
+FC
+FC
+FC
+MA
+crust
+</text>
+  </threadedComment>
+  <threadedComment ref="AC36" dT="2024-06-27T12:12:15.58" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{4BFCC566-92E8-4928-8748-52B17BD7C38D}">
+    <text>=Dref, Te=NA</text>
+  </threadedComment>
   <threadedComment ref="H38" dT="2024-04-30T15:19:22.86" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
     <text>Read from xs=0.05 on Fig3</text>
   </threadedComment>
@@ -2233,6 +2320,13 @@
     <text>Read from Fig2</text>
   </threadedComment>
   <threadedComment ref="T38" dT="2024-06-05T14:59:36.31" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{4805467D-952B-41B4-86D7-6B034FCD91D7}">
+    <text xml:space="preserve">Fe,liq
+Fe,sol
+Fe3S,sol
+FeSV,sol
+</text>
+  </threadedComment>
+  <threadedComment ref="AB38" dT="2024-06-05T14:59:36.31" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{A4073D4E-E1DC-44B0-9181-10733F210188}">
     <text xml:space="preserve">Fe,liq
 Fe,sol
 Fe3S,sol
@@ -2304,40 +2398,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB330E3-6480-4A3B-99B7-DBDC59EB106C}">
-  <dimension ref="B2:AK54"/>
+  <dimension ref="B2:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AK15" sqref="AK15"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="19"/>
-    <col min="3" max="4" width="8.88671875" style="17"/>
-    <col min="5" max="5" width="8.88671875" style="18"/>
-    <col min="7" max="7" width="8.88671875" style="19"/>
-    <col min="8" max="9" width="8.88671875" style="17"/>
-    <col min="10" max="10" width="8.88671875" style="18"/>
-    <col min="12" max="12" width="8.88671875" style="19"/>
-    <col min="13" max="17" width="8.88671875" style="17"/>
-    <col min="18" max="18" width="8.88671875" style="18"/>
+    <col min="2" max="2" width="8.88671875" style="16"/>
+    <col min="5" max="5" width="8.88671875" style="15"/>
+    <col min="7" max="7" width="8.88671875" style="16"/>
+    <col min="10" max="10" width="8.88671875" style="15"/>
+    <col min="12" max="12" width="8.88671875" style="16"/>
+    <col min="18" max="18" width="8.88671875" style="15"/>
     <col min="31" max="31" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="14" t="s">
         <v>128</v>
       </c>
       <c r="T2" s="1" t="s">
@@ -2347,60 +2438,61 @@
         <v>201</v>
       </c>
       <c r="AI2" s="1"/>
-    </row>
-    <row r="3" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+      <c r="AM2" s="1"/>
+    </row>
+    <row r="3" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B3" s="14"/>
+      <c r="C3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" t="s">
         <v>103</v>
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4">
         <v>2439</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4">
         <f>2439</f>
         <v>2439</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="1" t="s">
         <v>95</v>
       </c>
       <c r="T4" s="1" t="s">
@@ -2440,43 +2532,43 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5">
         <f>3302*10^(20)</f>
         <v>3.3019999999999999E+23</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5">
         <f>3.302E+23</f>
         <v>3.3019999999999999E+23</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" t="s">
         <v>133</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5">
         <v>0.33010299999999998</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O5">
         <v>2.0999999999999999E-5</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" t="s">
         <v>134</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" t="s">
         <v>135</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="R5" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="13"/>
+      <c r="S5" s="12"/>
       <c r="T5" t="s">
         <v>132</v>
       </c>
@@ -2495,7 +2587,7 @@
       <c r="Y5" t="s">
         <v>135</v>
       </c>
-      <c r="Z5" s="13" t="s">
+      <c r="Z5" s="12" t="s">
         <v>136</v>
       </c>
       <c r="AB5" t="s">
@@ -2516,42 +2608,42 @@
       <c r="AG5" t="s">
         <v>135</v>
       </c>
-      <c r="AH5" s="13" t="s">
+      <c r="AH5" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6">
         <v>5430</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6">
         <v>5434</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" t="s">
         <v>138</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6">
         <v>2439.4</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6">
         <v>0.1</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="P6" t="s">
         <v>139</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" t="s">
         <v>140</v>
       </c>
       <c r="T6" t="s">
@@ -2591,29 +2683,29 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B7" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" t="s">
         <v>142</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7">
         <v>0.34599999999999997</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7">
         <v>1.4E-2</v>
       </c>
-      <c r="P7" s="25" t="s">
+      <c r="P7" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="Q7" s="17" t="s">
+      <c r="Q7" t="s">
         <v>144</v>
       </c>
       <c r="T7" t="s">
@@ -2628,7 +2720,7 @@
       <c r="W7">
         <v>1.4E-2</v>
       </c>
-      <c r="X7" s="14" t="s">
+      <c r="X7" s="13" t="s">
         <v>143</v>
       </c>
       <c r="Y7" t="s">
@@ -2646,44 +2738,44 @@
       <c r="AE7">
         <v>1.4E-2</v>
       </c>
-      <c r="AF7" s="14" t="s">
+      <c r="AF7" s="13" t="s">
         <v>143</v>
       </c>
       <c r="AG7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B8" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8">
         <f>-0.00006</f>
         <v>-6.0000000000000002E-5</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8">
         <f>0.00002</f>
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" t="s">
         <v>145</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8">
         <v>0.43099999999999999</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="P8" s="25" t="s">
+      <c r="P8" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="Q8" s="17" t="s">
+      <c r="Q8" t="s">
         <v>144</v>
       </c>
       <c r="T8" t="s">
@@ -2698,7 +2790,7 @@
       <c r="W8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="X8" s="14" t="s">
+      <c r="X8" s="13" t="s">
         <v>143</v>
       </c>
       <c r="Y8" t="s">
@@ -2716,26 +2808,26 @@
       <c r="AE8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AF8" s="14" t="s">
+      <c r="AF8" s="13" t="s">
         <v>143</v>
       </c>
       <c r="AG8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9">
         <f>0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9">
         <f>0.000005</f>
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="16" t="s">
         <v>109</v>
       </c>
       <c r="AC9" t="s">
@@ -2745,35 +2837,35 @@
         <v>1.22</v>
       </c>
       <c r="AG9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10">
         <v>58.6462</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="P10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="Q10" s="1" t="s">
         <v>95</v>
       </c>
       <c r="T10" s="1" t="s">
@@ -2786,26 +2878,26 @@
         <v>0.8</v>
       </c>
       <c r="AG10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="L11" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="L11" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" t="s">
         <v>149</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11">
         <v>2900</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11">
         <v>3300</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" t="s">
         <v>150</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="Q11">
         <v>4</v>
       </c>
       <c r="AC11" t="s">
@@ -2815,26 +2907,26 @@
         <v>0.54</v>
       </c>
       <c r="AG11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="L12" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="L12" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" t="s">
         <v>152</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12">
         <v>50</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12">
         <v>200</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" t="s">
         <v>139</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" t="s">
         <v>153</v>
       </c>
       <c r="AC12" t="s">
@@ -2844,26 +2936,26 @@
         <v>0.65</v>
       </c>
       <c r="AG12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="L13" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="L13" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" t="s">
         <v>155</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13">
         <v>2350</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13">
         <v>2550</v>
       </c>
-      <c r="P13" s="17" t="s">
+      <c r="P13" t="s">
         <v>156</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" t="s">
         <v>157</v>
       </c>
       <c r="AC13" t="s">
@@ -2873,2041 +2965,2112 @@
         <v>0.36</v>
       </c>
       <c r="AG13" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" t="s">
         <v>155</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14">
         <f>N13</f>
         <v>2350</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14">
         <f>O13</f>
         <v>2550</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="P14" t="s">
         <v>156</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" t="s">
         <v>159</v>
       </c>
-      <c r="AC14" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD14">
-        <v>0.44</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+    </row>
+    <row r="15" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15">
         <v>2440</v>
       </c>
-      <c r="D15" s="17">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15">
         <v>2439</v>
       </c>
-      <c r="J15" s="18">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19" t="s">
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="M15" t="s">
         <v>161</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15">
         <v>1600</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15">
         <v>2000</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="P15" t="s">
         <v>156</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" t="s">
         <v>162</v>
       </c>
-      <c r="AC15" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD15">
-        <v>0.8</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="AB15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="1">
         <v>1860</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16">
         <v>7.5</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="15">
         <v>3350</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="4">
         <f>H15-100</f>
         <v>2339</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="M16" s="17" t="s">
+      <c r="M16" t="s">
         <v>164</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16">
         <v>-180</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16">
         <v>430</v>
       </c>
-      <c r="P16" s="17" t="s">
+      <c r="P16" t="s">
         <v>165</v>
       </c>
-      <c r="Q16" s="17" t="s">
+      <c r="Q16" t="s">
         <v>166</v>
       </c>
-      <c r="R16" s="18" t="s">
+      <c r="R16" s="15" t="s">
         <v>167</v>
       </c>
+      <c r="AB16" t="s">
+        <v>198</v>
+      </c>
       <c r="AC16" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
       <c r="AD16">
-        <v>0.45100000000000001</v>
-      </c>
-      <c r="AE16">
-        <v>1.4E-2</v>
+        <f>10^5</f>
+        <v>100000</v>
       </c>
       <c r="AF16" t="s">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="AG16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="17">
-        <v>0</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>39</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <v>8000</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" t="s">
         <v>121</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17">
         <f>N16+273.15</f>
         <v>93.149999999999977</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17">
         <f>O16+273.15</f>
         <v>703.15</v>
       </c>
-    </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G18" s="19" t="s">
+      <c r="AB17" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD17">
+        <v>3.3</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G18" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="1">
         <v>1790</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="U18" s="15" t="s">
+      <c r="U18" t="s">
         <v>191</v>
       </c>
-      <c r="V18" s="15" t="s">
+      <c r="V18" t="s">
         <v>113</v>
       </c>
-      <c r="W18" s="15" t="s">
+      <c r="W18" t="s">
         <v>92</v>
       </c>
-      <c r="X18" s="15" t="s">
+      <c r="X18" t="s">
         <v>192</v>
       </c>
-      <c r="Y18" s="15" t="s">
+      <c r="Y18" t="s">
         <v>183</v>
       </c>
-      <c r="Z18" s="15"/>
-      <c r="AB18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF18" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AG18" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G19" s="19" t="s">
+      <c r="AB18" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD18">
+        <f>10^18</f>
+        <v>1E+18</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>214</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G19" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H19" s="17">
-        <v>0</v>
-      </c>
-      <c r="J19" s="23">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
         <v>8000</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="M19" s="21" t="s">
+      <c r="M19" t="s">
         <v>104</v>
       </c>
-      <c r="N19" s="17" t="s">
+      <c r="N19" t="s">
         <v>113</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" t="s">
         <v>106</v>
       </c>
-      <c r="T19" s="15" t="s">
+      <c r="T19" t="s">
         <v>71</v>
       </c>
-      <c r="U19" s="15">
-        <v>0</v>
-      </c>
-      <c r="V19" s="15">
-        <v>0</v>
-      </c>
-      <c r="W19" s="15">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
         <f>AVERAGE(2900,3100)</f>
         <v>3000</v>
       </c>
-      <c r="X19" s="15">
+      <c r="X19">
         <v>398.15</v>
       </c>
-      <c r="Y19" s="15">
+      <c r="Y19">
         <f>VLOOKUP($T19,MatExport[#All],7,FALSE)
 +VLOOKUP($T19,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T19,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>120</v>
       </c>
-      <c r="Z19" s="15"/>
       <c r="AB19" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="AC19" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="AD19">
-        <f>10^5</f>
-        <v>100000</v>
+        <v>70</v>
       </c>
       <c r="AF19" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="AG19" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+    <row r="20" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="19" t="s">
+      <c r="L20" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="M20" s="17" t="str">
+      <c r="M20" t="str">
         <f>M13</f>
         <v>T_core</v>
       </c>
-      <c r="O20" s="17">
-        <v>0</v>
-      </c>
-      <c r="T20" s="15" t="s">
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
         <v>89</v>
       </c>
       <c r="U20" s="1">
         <v>43.1</v>
       </c>
-      <c r="V20" s="15">
+      <c r="V20">
         <v>1.4930000000000001</v>
       </c>
-      <c r="W20" s="15">
+      <c r="W20">
         <f>VLOOKUP(T20,MatExport[],4,FALSE)</f>
         <v>3307.6</v>
       </c>
-      <c r="X20" s="15">
+      <c r="X20">
         <v>1099.75</v>
       </c>
-      <c r="Y20" s="15">
+      <c r="Y20">
         <f>VLOOKUP($T20,MatExport[#All],7,FALSE)
 +VLOOKUP($T20,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T20,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-      <c r="Z20" s="15"/>
       <c r="AB20" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="AC20" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="AD20">
-        <v>3.3</v>
+        <f>10^20</f>
+        <v>1E+20</v>
       </c>
       <c r="AF20" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="AG20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+    <row r="21" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B21" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21">
         <v>2440</v>
       </c>
-      <c r="D21" s="17">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="G21" s="16" t="s">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" t="s">
         <v>113</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M21" s="17" t="str">
+      <c r="M21" t="str">
         <f>M14</f>
         <v>T_core</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21">
         <v>2900</v>
       </c>
-      <c r="T21" s="15" t="s">
+      <c r="T21" t="s">
         <v>85</v>
       </c>
-      <c r="U21" s="15">
+      <c r="U21">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
         <v>2011.0545999999999</v>
       </c>
-      <c r="V21" s="15">
+      <c r="V21">
         <v>2.4287999999999998</v>
       </c>
-      <c r="W21" s="15">
+      <c r="W21">
         <f>VLOOKUP(T21,MatExport[],4,FALSE)</f>
         <v>7019</v>
       </c>
-      <c r="X21" s="15">
+      <c r="X21">
         <v>1800</v>
       </c>
-      <c r="Y21" s="15">
+      <c r="Y21">
         <f>VLOOKUP($T21,MatExport[#All],7,FALSE)
 +VLOOKUP($T21,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T21,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>-862.70086415590015</v>
       </c>
-      <c r="Z21" s="15"/>
-      <c r="AB21" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD21">
-        <f>10^18</f>
-        <v>1E+18</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
+    </row>
+    <row r="22" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="15">
         <v>3590</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22">
         <f>H15</f>
         <v>2439</v>
       </c>
-      <c r="J22" s="18">
-        <v>0</v>
-      </c>
-      <c r="L22" s="19" t="s">
+      <c r="J22" s="15">
+        <v>0</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="10">
         <v>2011.0545999999999</v>
       </c>
-      <c r="O22" s="17">
+      <c r="O22">
         <v>3400</v>
       </c>
-      <c r="T22" s="15" t="s">
+      <c r="T22" t="s">
         <v>55</v>
       </c>
-      <c r="U22" s="15">
+      <c r="U22">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
         <v>1342.6297999999999</v>
       </c>
-      <c r="V22" s="15">
+      <c r="V22">
         <v>21.718399999999999</v>
       </c>
-      <c r="W22" s="15">
+      <c r="W22">
         <f>VLOOKUP(T22,MatExport[],4,FALSE)</f>
         <v>7225</v>
       </c>
-      <c r="X22" s="15">
+      <c r="X22">
         <v>2450</v>
       </c>
-      <c r="Y22" s="15">
+      <c r="Y22">
         <f>VLOOKUP($T22,MatExport[#All],7,FALSE)
 +VLOOKUP($T22,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T22,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>127</v>
       </c>
-      <c r="Z22" s="15"/>
-      <c r="AB22" t="s">
-        <v>215</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>216</v>
-      </c>
-      <c r="AD22">
-        <v>70</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>211</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
+      <c r="AB22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23">
         <f>0.7*C21</f>
         <v>1708</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="15">
         <v>5450</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23">
         <f>H16</f>
         <v>2339</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="15">
         <v>2900</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="10">
         <v>1342.6297999999999</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="10">
         <v>4.3327999999999998</v>
       </c>
-      <c r="O23" s="17">
+      <c r="O23">
         <v>3700</v>
       </c>
-      <c r="T23" s="15" t="s">
+      <c r="T23" t="s">
         <v>180</v>
       </c>
-      <c r="U23" s="15">
+      <c r="U23">
         <f>2439.4</f>
         <v>2439.4</v>
       </c>
-      <c r="V23" s="15">
+      <c r="V23">
         <v>34.403199999999998</v>
       </c>
-      <c r="W23" s="15" t="s">
+      <c r="W23" t="s">
         <v>182</v>
       </c>
-      <c r="X23" s="15">
+      <c r="X23">
         <v>2450</v>
       </c>
-      <c r="Y23" s="15" t="s">
+      <c r="Y23" t="s">
         <v>182</v>
       </c>
-      <c r="AB23" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>217</v>
-      </c>
-      <c r="AD23">
-        <f>10^20</f>
-        <v>1E+20</v>
+      <c r="AC23">
+        <v>0.44</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE23">
+        <v>0.8</v>
       </c>
       <c r="AF23" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="AG23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B24" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="17">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
         <v>8000</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24">
         <v>2040</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="15">
         <v>3400</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="M24" s="17">
-        <v>0</v>
-      </c>
-      <c r="N24" s="12">
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="11">
         <v>35.403199999999998</v>
       </c>
-      <c r="O24" s="17">
+      <c r="O24">
         <f>O17</f>
         <v>703.15</v>
       </c>
-      <c r="T24" s="15" t="s">
+      <c r="T24" t="s">
         <v>178</v>
       </c>
-      <c r="U24" s="15">
+      <c r="U24">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
         <v>5.1595000000000004</v>
       </c>
-      <c r="V24" s="15" t="s">
+      <c r="V24" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G25" s="19" t="s">
+      <c r="AC24">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="AD24">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G25" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H25" s="17">
+      <c r="H25">
         <f>H18</f>
         <v>1790</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="15">
         <v>3700</v>
       </c>
-    </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G26" s="19" t="s">
+      <c r="AJ25" t="s">
+        <v>232</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G26" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H26" s="17">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="15">
         <f>J19</f>
         <v>8000</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="U26" s="15" t="s">
+      <c r="U26" t="s">
         <v>191</v>
       </c>
-      <c r="V26" s="15" t="s">
+      <c r="V26" t="s">
         <v>113</v>
       </c>
-      <c r="W26" s="15" t="s">
+      <c r="W26" t="s">
         <v>92</v>
       </c>
-      <c r="X26" s="15" t="s">
+      <c r="X26" t="s">
         <v>192</v>
       </c>
-      <c r="Y26" s="15" t="s">
+      <c r="Y26" t="s">
         <v>183</v>
       </c>
-      <c r="Z26" s="15"/>
-      <c r="AB26" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AC26" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD26" s="15" t="s">
+      <c r="AC26">
+        <f>AVERAGE(0.3,0.45)</f>
+        <v>0.375</v>
+      </c>
+      <c r="AD26">
+        <f>(0.45-0.3)/2</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="AE26">
+        <f>AVERAGE(0.6,0.8)</f>
+        <v>0.7</v>
+      </c>
+      <c r="AF26">
+        <f>(0.8-0.6)/2</f>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="L27" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="M27" t="s">
+        <v>104</v>
+      </c>
+      <c r="N27" t="s">
         <v>113</v>
       </c>
-      <c r="AE26" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF26" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG26" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH26" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI26" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="L27" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="M27" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="N27" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="O27" s="21" t="s">
+      <c r="O27" t="s">
         <v>106</v>
       </c>
-      <c r="P27" s="21" t="s">
+      <c r="P27" t="s">
         <v>181</v>
       </c>
-      <c r="Q27" s="21" t="s">
+      <c r="Q27" t="s">
         <v>183</v>
       </c>
-      <c r="R27" s="26"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15" t="s">
+      <c r="T27" t="s">
         <v>71</v>
       </c>
-      <c r="U27" s="15">
-        <v>0</v>
-      </c>
-      <c r="V27" s="15">
-        <v>0</v>
-      </c>
-      <c r="W27" s="15">
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
         <f>AVERAGE(2900,3100)</f>
         <v>3000</v>
       </c>
-      <c r="X27" s="15">
+      <c r="X27">
         <v>398.15</v>
       </c>
-      <c r="Y27" s="15">
+      <c r="Y27">
         <f>VLOOKUP($T27,MatExport[#All],7,FALSE)
 +VLOOKUP($T27,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T27,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>120</v>
       </c>
-      <c r="Z27" s="15"/>
-      <c r="AB27" s="15" t="s">
+      <c r="AC27">
+        <f>AVERAGE(0.3,0.4)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AD27">
+        <f>(0.4-0)/2</f>
+        <v>0.2</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G28" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AC27" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="5">
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>AVERAGE(2900,3100)</f>
+        <v>3000</v>
+      </c>
+      <c r="P28">
+        <v>398.15</v>
+      </c>
+      <c r="Q28">
+        <f>VLOOKUP(L28,MatExport[#All],7,FALSE)
++VLOOKUP(L28,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP(L28,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>120</v>
+      </c>
+      <c r="T28" t="s">
+        <v>89</v>
+      </c>
+      <c r="U28" s="1">
+        <v>108.43</v>
+      </c>
+      <c r="V28">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="W28">
+        <f>VLOOKUP(T28,MatExport[],4,FALSE)</f>
+        <v>3307.6</v>
+      </c>
+      <c r="X28">
+        <v>1099.75</v>
+      </c>
+      <c r="Y28">
+        <f>VLOOKUP($T28,MatExport[#All],7,FALSE)
++VLOOKUP($T28,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T28,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>129.89999999999998</v>
+      </c>
+      <c r="AC28">
+        <f>AVERAGE(0.25,0.75)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AD28">
+        <f>(0.75-0.25)/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="AE28">
+        <f>AVERAGE(0.5,1.3)</f>
+        <v>0.9</v>
+      </c>
+      <c r="AF28">
+        <f>(1.3-0.5)/2</f>
+        <v>0.4</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G29" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29">
+        <f>H22</f>
+        <v>2439</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29">
+        <f>AVERAGE(50,200)</f>
+        <v>125</v>
+      </c>
+      <c r="N29">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="O29">
+        <f>VLOOKUP(L29,MatExport[],4,FALSE)</f>
+        <v>3307.6</v>
+      </c>
+      <c r="P29">
+        <v>1099.75</v>
+      </c>
+      <c r="Q29">
+        <f>VLOOKUP(L29,MatExport[#All],7,FALSE)
++VLOOKUP(L29,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP(L29,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>129.89999999999998</v>
+      </c>
+      <c r="T29" t="s">
+        <v>85</v>
+      </c>
+      <c r="U29">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
+        <v>2011.0545999999999</v>
+      </c>
+      <c r="V29">
+        <v>2.4287999999999998</v>
+      </c>
+      <c r="W29">
+        <f>VLOOKUP(T29,MatExport[],4,FALSE)</f>
+        <v>7019</v>
+      </c>
+      <c r="X29">
+        <v>1800</v>
+      </c>
+      <c r="Y29">
+        <f>VLOOKUP($T29,MatExport[#All],7,FALSE)
++VLOOKUP($T29,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T29,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>-862.70086415590015</v>
+      </c>
+      <c r="AC29">
+        <f>AVERAGE(0.4,0.425)</f>
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="AD29">
+        <f>(0.425-0.4)/2</f>
+        <v>1.2499999999999983E-2</v>
+      </c>
+      <c r="AE29">
+        <f>AVERAGE(0.75,0.9)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="AF29">
+        <f>(0.9-0.75)/2</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G30" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30">
+        <f>H23</f>
+        <v>2339</v>
+      </c>
+      <c r="J30" s="15">
+        <v>2900</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="M30">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
+        <v>2011.0545999999999</v>
+      </c>
+      <c r="N30">
+        <v>2.4287999999999998</v>
+      </c>
+      <c r="O30">
+        <f>VLOOKUP(L30,MatExport[],4,FALSE)</f>
+        <v>7019</v>
+      </c>
+      <c r="P30">
+        <v>1800</v>
+      </c>
+      <c r="Q30">
+        <f>VLOOKUP(L30,MatExport[#All],7,FALSE)
++VLOOKUP(L30,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP(L30,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>-862.70086415590015</v>
+      </c>
+      <c r="T30" t="s">
+        <v>55</v>
+      </c>
+      <c r="U30">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
+        <v>1342.6297999999999</v>
+      </c>
+      <c r="V30">
+        <v>21.718399999999999</v>
+      </c>
+      <c r="W30">
+        <f>VLOOKUP(T30,MatExport[],4,FALSE)</f>
+        <v>7225</v>
+      </c>
+      <c r="X30">
+        <v>2450</v>
+      </c>
+      <c r="Y30">
+        <f>VLOOKUP($T30,MatExport[#All],7,FALSE)
++VLOOKUP($T30,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T30,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31">
+        <v>2050</v>
+      </c>
+      <c r="J31" s="15">
+        <v>3320</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M31">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
+        <v>1342.6297999999999</v>
+      </c>
+      <c r="N31">
+        <v>21.718399999999999</v>
+      </c>
+      <c r="O31">
+        <f>VLOOKUP(L31,MatExport[],4,FALSE)</f>
+        <v>7225</v>
+      </c>
+      <c r="P31">
+        <v>2450</v>
+      </c>
+      <c r="Q31">
+        <f>VLOOKUP(L31,MatExport[#All],7,FALSE)
++VLOOKUP(L31,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP(L31,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>127</v>
+      </c>
+      <c r="T31" t="s">
+        <v>180</v>
+      </c>
+      <c r="U31">
+        <f>2439.4</f>
+        <v>2439.4</v>
+      </c>
+      <c r="V31">
+        <v>34.403199999999998</v>
+      </c>
+      <c r="W31" t="s">
+        <v>182</v>
+      </c>
+      <c r="X31">
+        <v>2450</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="G32" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32">
+        <f>H25</f>
+        <v>1790</v>
+      </c>
+      <c r="J32" s="15">
+        <v>3420</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M32">
+        <f>2439.4</f>
+        <v>2439.4</v>
+      </c>
+      <c r="N32">
+        <v>34.403199999999998</v>
+      </c>
+      <c r="O32" t="s">
+        <v>182</v>
+      </c>
+      <c r="P32">
+        <v>2450</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>182</v>
+      </c>
+      <c r="T32" t="s">
+        <v>178</v>
+      </c>
+      <c r="U32">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
+        <v>5.1595000000000004</v>
+      </c>
+      <c r="V32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G33" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="J33" s="15">
+        <f>J26</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="34" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="L34" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="M34">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
+        <v>5.1595000000000004</v>
+      </c>
+      <c r="N34" t="s">
+        <v>179</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U34" t="s">
+        <v>191</v>
+      </c>
+      <c r="V34" t="s">
+        <v>113</v>
+      </c>
+      <c r="W34" t="s">
+        <v>92</v>
+      </c>
+      <c r="X34" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G35" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I35" t="s">
+        <v>113</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="T35" t="s">
+        <v>71</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <f>AVERAGE(2900,3100)</f>
+        <v>3000</v>
+      </c>
+      <c r="X35">
+        <v>398.15</v>
+      </c>
+      <c r="Y35">
+        <f>VLOOKUP($T35,MatExport[#All],7,FALSE)
++VLOOKUP($T35,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T35,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+        <v>120</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="5">
         <v>3100</v>
       </c>
-      <c r="AF27" s="15">
+      <c r="AF35">
         <v>398.15</v>
       </c>
-      <c r="AG27" s="15">
+      <c r="AG35">
         <f>VLOOKUP($T19,MatExport[#All],7,FALSE)
 +VLOOKUP($T19,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T19,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>120</v>
       </c>
-      <c r="AH27" s="5">
-        <f>$AD$22</f>
+      <c r="AH35" s="5">
+        <f>$AD$19</f>
         <v>70</v>
       </c>
-      <c r="AI27" s="15">
+      <c r="AI35">
         <f>10^23</f>
         <v>9.9999999999999992E+22</v>
       </c>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G28" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H28" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="L28" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="M28" s="21">
-        <v>0</v>
-      </c>
-      <c r="N28" s="21">
-        <v>0</v>
-      </c>
-      <c r="O28" s="21">
-        <f>AVERAGE(2900,3100)</f>
-        <v>3000</v>
-      </c>
-      <c r="P28" s="21">
-        <v>398.15</v>
-      </c>
-      <c r="Q28" s="21">
-        <f>VLOOKUP(L28,MatExport[#All],7,FALSE)
-+VLOOKUP(L28,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP(L28,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>120</v>
-      </c>
-      <c r="T28" s="15" t="s">
+    <row r="36" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G36" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H36">
+        <f>H29</f>
+        <v>2439</v>
+      </c>
+      <c r="J36" s="15">
+        <v>0</v>
+      </c>
+      <c r="T36" t="s">
         <v>89</v>
       </c>
-      <c r="U28" s="1">
-        <v>108.43</v>
-      </c>
-      <c r="V28" s="15">
+      <c r="U36" s="1">
+        <v>112.45399999999999</v>
+      </c>
+      <c r="V36">
         <v>1.4930000000000001</v>
       </c>
-      <c r="W28" s="15">
-        <f>VLOOKUP(T28,MatExport[],4,FALSE)</f>
+      <c r="W36">
+        <f>VLOOKUP(T36,MatExport[],4,FALSE)</f>
         <v>3307.6</v>
       </c>
-      <c r="X28" s="15">
+      <c r="X36">
         <v>1099.75</v>
       </c>
-      <c r="Y28" s="15">
-        <f>VLOOKUP($T28,MatExport[#All],7,FALSE)
-+VLOOKUP($T28,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T28,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+      <c r="Y36">
+        <f>VLOOKUP($T36,MatExport[#All],7,FALSE)
++VLOOKUP($T36,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T36,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-      <c r="Z28" s="15"/>
-      <c r="AB28" s="15" t="s">
+      <c r="AB36" t="s">
         <v>89</v>
       </c>
-      <c r="AC28" s="15">
+      <c r="AC36">
         <v>112.45399999999999</v>
       </c>
-      <c r="AD28" s="15">
+      <c r="AD36">
         <v>1.3422000000000001</v>
       </c>
-      <c r="AE28" s="15">
-        <f>VLOOKUP(AB28,MatExport[],4,FALSE)</f>
+      <c r="AE36">
+        <f>VLOOKUP(AB36,MatExport[],4,FALSE)</f>
         <v>3307.6</v>
       </c>
-      <c r="AF28" s="15">
+      <c r="AF36">
         <v>1099.75</v>
       </c>
-      <c r="AG28" s="15">
+      <c r="AG36">
         <f>VLOOKUP($T20,MatExport[#All],7,FALSE)
 +VLOOKUP($T20,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T20,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-      <c r="AH28" s="5">
-        <f>$AD$22</f>
+      <c r="AH36" s="5">
+        <f>$AD$19</f>
         <v>70</v>
       </c>
-      <c r="AI28" s="15">
-        <f>AD23</f>
+      <c r="AI36">
+        <f>AD20</f>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G29" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H29" s="17">
-        <f>H22</f>
-        <v>2439</v>
-      </c>
-      <c r="J29" s="18">
-        <v>0</v>
-      </c>
-      <c r="L29" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="M29" s="21">
-        <f>AVERAGE(50,200)</f>
-        <v>125</v>
-      </c>
-      <c r="N29" s="21">
-        <v>1.4930000000000001</v>
-      </c>
-      <c r="O29" s="21">
-        <f>VLOOKUP(L29,MatExport[],4,FALSE)</f>
-        <v>3307.6</v>
-      </c>
-      <c r="P29" s="21">
-        <v>1099.75</v>
-      </c>
-      <c r="Q29" s="21">
-        <f>VLOOKUP(L29,MatExport[#All],7,FALSE)
-+VLOOKUP(L29,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP(L29,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>129.89999999999998</v>
-      </c>
-      <c r="T29" s="15" t="s">
+    <row r="37" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G37" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37">
+        <f>H30</f>
+        <v>2339</v>
+      </c>
+      <c r="J37" s="15">
+        <v>2900</v>
+      </c>
+      <c r="T37" t="s">
         <v>85</v>
       </c>
-      <c r="U29" s="15">
+      <c r="U37">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
         <v>2011.0545999999999</v>
       </c>
-      <c r="V29" s="15">
+      <c r="V37">
         <v>2.4287999999999998</v>
       </c>
-      <c r="W29" s="15">
-        <f>VLOOKUP(T29,MatExport[],4,FALSE)</f>
+      <c r="W37">
+        <f>VLOOKUP(T37,MatExport[],4,FALSE)</f>
         <v>7019</v>
       </c>
-      <c r="X29" s="15">
+      <c r="X37">
         <v>1800</v>
       </c>
-      <c r="Y29" s="15">
-        <f>VLOOKUP($T29,MatExport[#All],7,FALSE)
-+VLOOKUP($T29,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T29,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+      <c r="Y37">
+        <f>VLOOKUP($T37,MatExport[#All],7,FALSE)
++VLOOKUP($T37,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T37,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>-862.70086415590015</v>
       </c>
-      <c r="Z29" s="15"/>
-      <c r="AB29" s="15" t="s">
+      <c r="AB37" t="s">
         <v>85</v>
       </c>
-      <c r="AC29" s="15">
+      <c r="AC37">
         <v>1326.0509999999999</v>
       </c>
-      <c r="AD29" s="15">
+      <c r="AD37">
         <v>4.3647</v>
       </c>
-      <c r="AE29" s="15">
-        <f>VLOOKUP(AB29,MatExport[],4,FALSE)</f>
+      <c r="AE37">
+        <f>VLOOKUP(AB37,MatExport[],4,FALSE)</f>
         <v>7019</v>
       </c>
-      <c r="AF29" s="15">
+      <c r="AF37">
         <v>1800</v>
       </c>
-      <c r="AG29" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH29" s="5">
-        <f>$AD$22</f>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="5">
+        <f>$AD$19</f>
         <v>70</v>
       </c>
-      <c r="AI29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G30" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H30" s="17">
-        <f>H23</f>
-        <v>2339</v>
-      </c>
-      <c r="J30" s="18">
-        <v>2900</v>
-      </c>
-      <c r="L30" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="M30" s="21">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
-        <v>2011.0545999999999</v>
-      </c>
-      <c r="N30" s="21">
-        <v>2.4287999999999998</v>
-      </c>
-      <c r="O30" s="21">
-        <f>VLOOKUP(L30,MatExport[],4,FALSE)</f>
-        <v>7019</v>
-      </c>
-      <c r="P30" s="21">
-        <v>1800</v>
-      </c>
-      <c r="Q30" s="21">
-        <f>VLOOKUP(L30,MatExport[#All],7,FALSE)
-+VLOOKUP(L30,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP(L30,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>-862.70086415590015</v>
-      </c>
-      <c r="T30" s="15" t="s">
+      <c r="AI37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G38" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38">
+        <v>2050</v>
+      </c>
+      <c r="J38" s="15">
+        <v>3360</v>
+      </c>
+      <c r="T38" t="s">
         <v>55</v>
       </c>
-      <c r="U30" s="15">
+      <c r="U38">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
         <v>1342.6297999999999</v>
       </c>
-      <c r="V30" s="15">
+      <c r="V38">
         <v>21.718399999999999</v>
       </c>
-      <c r="W30" s="15">
-        <f>VLOOKUP(T30,MatExport[],4,FALSE)</f>
+      <c r="W38">
+        <f>VLOOKUP(T38,MatExport[],4,FALSE)</f>
         <v>7225</v>
       </c>
-      <c r="X30" s="15">
+      <c r="X38">
         <v>2450</v>
       </c>
-      <c r="Y30" s="15">
-        <f>VLOOKUP($T30,MatExport[#All],7,FALSE)
-+VLOOKUP($T30,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T30,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
+      <c r="Y38">
+        <f>VLOOKUP($T38,MatExport[#All],7,FALSE)
++VLOOKUP($T38,MatExport[#All],5,FALSE)*($M$34/100)
++VLOOKUP($T38,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>127</v>
       </c>
-      <c r="Z30" s="15"/>
-      <c r="AB30" s="15" t="s">
+      <c r="AB38" t="s">
         <v>55</v>
       </c>
-      <c r="AC30" s="15">
+      <c r="AC38">
         <v>2011.5958000000001</v>
       </c>
-      <c r="AD30" s="15">
+      <c r="AD38">
         <v>21.886399999999998</v>
       </c>
-      <c r="AE30" s="15">
-        <f>VLOOKUP(AB30,MatExport[],4,FALSE)</f>
+      <c r="AE38">
+        <f>VLOOKUP(AB38,MatExport[],4,FALSE)</f>
         <v>7225</v>
       </c>
-      <c r="AF30" s="15">
+      <c r="AF38">
         <v>2450</v>
       </c>
-      <c r="AG30" s="15">
+      <c r="AG38">
         <f>VLOOKUP($T22,MatExport[#All],7,FALSE)
 +VLOOKUP($T22,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T22,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>127</v>
       </c>
-      <c r="AH30" s="5">
-        <f>$AD$22</f>
+      <c r="AH38" s="5">
+        <f>$AD$19</f>
         <v>70</v>
       </c>
-      <c r="AI30" s="15">
+      <c r="AI38">
         <f>10^20</f>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G31" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="17">
-        <v>2050</v>
-      </c>
-      <c r="J31" s="18">
-        <v>3320</v>
-      </c>
-      <c r="L31" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="M31" s="21">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
-        <v>1342.6297999999999</v>
-      </c>
-      <c r="N31" s="21">
-        <v>21.718399999999999</v>
-      </c>
-      <c r="O31" s="21">
-        <f>VLOOKUP(L31,MatExport[],4,FALSE)</f>
-        <v>7225</v>
-      </c>
-      <c r="P31" s="21">
-        <v>2450</v>
-      </c>
-      <c r="Q31" s="21">
-        <f>VLOOKUP(L31,MatExport[#All],7,FALSE)
-+VLOOKUP(L31,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP(L31,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>127</v>
-      </c>
-      <c r="T31" s="15" t="s">
+    <row r="39" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G39" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H39">
+        <f>H32</f>
+        <v>1790</v>
+      </c>
+      <c r="J39" s="15">
+        <v>3520</v>
+      </c>
+      <c r="T39" t="s">
         <v>180</v>
       </c>
-      <c r="U31" s="15">
+      <c r="U39">
         <f>2439.4</f>
         <v>2439.4</v>
       </c>
-      <c r="V31" s="15">
+      <c r="V39">
         <v>34.403199999999998</v>
       </c>
-      <c r="W31" s="15" t="s">
+      <c r="W39" t="s">
         <v>182</v>
       </c>
-      <c r="X31" s="15">
+      <c r="X39">
         <v>2450</v>
       </c>
-      <c r="Y31" s="15" t="s">
+      <c r="Y39" t="s">
         <v>182</v>
       </c>
-      <c r="AB31" s="15" t="s">
+      <c r="AB39" t="s">
         <v>180</v>
       </c>
-      <c r="AC31" s="15">
+      <c r="AC39">
         <f>2439.4</f>
         <v>2439.4</v>
       </c>
-      <c r="AD31" s="15">
+      <c r="AD39">
         <v>35.418999999999997</v>
       </c>
-      <c r="AE31" s="15" t="s">
+      <c r="AE39" t="s">
         <v>182</v>
       </c>
-      <c r="AF31" s="15">
+      <c r="AF39">
         <v>2450</v>
       </c>
-      <c r="AG31" s="15" t="s">
+      <c r="AG39" t="s">
         <v>182</v>
       </c>
-      <c r="AH31" t="s">
+      <c r="AH39" t="s">
         <v>182</v>
       </c>
-      <c r="AI31" t="s">
+      <c r="AI39" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="G32" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" s="17">
-        <f>H25</f>
-        <v>1790</v>
-      </c>
-      <c r="J32" s="18">
-        <v>3420</v>
-      </c>
-      <c r="L32" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="M32" s="21">
-        <f>2439.4</f>
-        <v>2439.4</v>
-      </c>
-      <c r="N32" s="21">
-        <v>34.403199999999998</v>
-      </c>
-      <c r="O32" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="P32" s="21">
-        <v>2450</v>
-      </c>
-      <c r="Q32" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="T32" s="15" t="s">
+    <row r="40" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G40" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="J40" s="15">
+        <f>J33</f>
+        <v>8000</v>
+      </c>
+      <c r="T40" t="s">
         <v>178</v>
       </c>
-      <c r="U32" s="15">
+      <c r="U40">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
         <v>5.1595000000000004</v>
       </c>
-      <c r="V32" s="15" t="s">
+      <c r="V40" t="s">
         <v>179</v>
       </c>
-      <c r="AB32" s="15" t="s">
+      <c r="AB40" t="s">
         <v>178</v>
       </c>
-      <c r="AC32" s="15">
+      <c r="AC40">
         <v>5.2923999999999998</v>
       </c>
-      <c r="AD32" s="15" t="s">
+      <c r="AD40" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G33" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H33" s="17">
-        <v>0</v>
-      </c>
-      <c r="J33" s="18">
-        <f>J26</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="34" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="L34" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="M34" s="17">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
-        <v>5.1595000000000004</v>
-      </c>
-      <c r="N34" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="U34" s="15" t="s">
+    <row r="42" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G42" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H42" t="s">
+        <v>104</v>
+      </c>
+      <c r="I42" t="s">
+        <v>113</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="U42" t="s">
         <v>191</v>
       </c>
-      <c r="V34" s="15" t="s">
+      <c r="V42" t="s">
         <v>113</v>
       </c>
-      <c r="W34" s="15" t="s">
+      <c r="W42" t="s">
         <v>92</v>
       </c>
-      <c r="X34" s="15" t="s">
+      <c r="X42" t="s">
         <v>192</v>
       </c>
-      <c r="Y34" s="15" t="s">
+      <c r="Y42" t="s">
         <v>183</v>
       </c>
-      <c r="AB34" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC34" s="15" t="s">
+      <c r="AB42" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC42" t="s">
         <v>191</v>
       </c>
-      <c r="AD34" s="15" t="s">
+      <c r="AD42" t="s">
         <v>113</v>
       </c>
-      <c r="AE34" s="15" t="s">
+      <c r="AE42" t="s">
         <v>92</v>
       </c>
-      <c r="AF34" s="15" t="s">
+      <c r="AF42" t="s">
         <v>192</v>
       </c>
-      <c r="AG34" s="15" t="s">
+      <c r="AG42" t="s">
         <v>208</v>
       </c>
-      <c r="AH34" s="15" t="s">
+      <c r="AH42" t="s">
         <v>209</v>
       </c>
-      <c r="AI34" s="15" t="s">
+      <c r="AI42" t="s">
         <v>193</v>
       </c>
-      <c r="AJ34" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="AK34" s="15" t="s">
+      <c r="AJ42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G35" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="T35" s="15" t="s">
+    <row r="43" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G43" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H43">
+        <f>H50</f>
+        <v>2439</v>
+      </c>
+      <c r="J43" s="15">
+        <v>0</v>
+      </c>
+      <c r="T43" t="s">
         <v>71</v>
       </c>
-      <c r="U35" s="15">
-        <v>0</v>
-      </c>
-      <c r="V35" s="15">
-        <v>0</v>
-      </c>
-      <c r="W35" s="15">
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
         <f>AVERAGE(2900,3100)</f>
         <v>3000</v>
       </c>
-      <c r="X35" s="15">
+      <c r="X43">
         <v>398.15</v>
       </c>
-      <c r="Y35" s="15">
-        <f>VLOOKUP($T35,MatExport[#All],7,FALSE)
-+VLOOKUP($T35,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T35,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>120</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC35">
-        <f>AC31</f>
-        <v>2439.4</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE35">
-        <f>AE27*(($AC28-$AC27)/$AC$31)^3+AE28*(($AC29-$AC28)/$AC$31)^3+AE29*(($AC30-$AC28)/$AC$31)^3+AE30*(($AC31-$AC30)/$AC$31)^3</f>
-        <v>3758.6090581055701</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG35">
-        <f>AG27*(($AC28-$AC27)/$AC$31)^3+AG28*(($AC29-$AC28)/$AC$31)^3+AG29*(($AC30-$AC28)/$AC$31)^3+AG30*(($AC31-$AC30)/$AC$31)^3</f>
-        <v>16.691730056956946</v>
-      </c>
-      <c r="AH35">
-        <f>AH27*(($AC28-$AC27)/$AC$31)^3+AH28*(($AC29-$AC28)/$AC$31)^3+AH29*(($AC30-$AC28)/$AC$31)^3+AH30*(($AC31-$AC30)/$AC$31)^3</f>
-        <v>42.034682506824353</v>
-      </c>
-    </row>
-    <row r="36" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G36" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H36" s="17">
-        <f>H29</f>
-        <v>2439</v>
-      </c>
-      <c r="J36" s="18">
-        <v>0</v>
-      </c>
-      <c r="T36" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="U36" s="1">
-        <v>112.45399999999999</v>
-      </c>
-      <c r="V36" s="15">
-        <v>1.4930000000000001</v>
-      </c>
-      <c r="W36" s="15">
-        <f>VLOOKUP(T36,MatExport[],4,FALSE)</f>
-        <v>3307.6</v>
-      </c>
-      <c r="X36" s="15">
-        <v>1099.75</v>
-      </c>
-      <c r="Y36" s="15">
-        <f>VLOOKUP($T36,MatExport[#All],7,FALSE)
-+VLOOKUP($T36,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T36,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>129.89999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" s="17">
-        <f>H30</f>
-        <v>2339</v>
-      </c>
-      <c r="J37" s="18">
-        <v>2900</v>
-      </c>
-      <c r="T37" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="U37" s="15">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
-        <v>2011.0545999999999</v>
-      </c>
-      <c r="V37" s="15">
-        <v>2.4287999999999998</v>
-      </c>
-      <c r="W37" s="15">
-        <f>VLOOKUP(T37,MatExport[],4,FALSE)</f>
-        <v>7019</v>
-      </c>
-      <c r="X37" s="15">
-        <v>1800</v>
-      </c>
-      <c r="Y37" s="15">
-        <f>VLOOKUP($T37,MatExport[#All],7,FALSE)
-+VLOOKUP($T37,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T37,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>-862.70086415590015</v>
-      </c>
-      <c r="AB37" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="AC37" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD37" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE37" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF37" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG37" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH37" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI37" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="AJ37" s="15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G38" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H38" s="17">
-        <v>2050</v>
-      </c>
-      <c r="J38" s="18">
-        <v>3360</v>
-      </c>
-      <c r="T38" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="U38" s="15">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
-        <v>1342.6297999999999</v>
-      </c>
-      <c r="V38" s="15">
-        <v>21.718399999999999</v>
-      </c>
-      <c r="W38" s="15">
-        <f>VLOOKUP(T38,MatExport[],4,FALSE)</f>
-        <v>7225</v>
-      </c>
-      <c r="X38" s="15">
-        <v>2450</v>
-      </c>
-      <c r="Y38" s="15">
-        <f>VLOOKUP($T38,MatExport[#All],7,FALSE)
-+VLOOKUP($T38,MatExport[#All],5,FALSE)*($M$34/100)
-+VLOOKUP($T38,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
-        <v>127</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC38">
-        <f>AC35</f>
-        <v>2439.4</v>
-      </c>
-      <c r="AD38" t="str">
-        <f t="shared" ref="AD38:AH38" si="0">AD35</f>
-        <v>NA</v>
-      </c>
-      <c r="AE38">
-        <f t="shared" si="0"/>
-        <v>3758.6090581055701</v>
-      </c>
-      <c r="AF38" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
-      </c>
-      <c r="AG38">
-        <f t="shared" si="0"/>
-        <v>16.691730056956946</v>
-      </c>
-      <c r="AH38">
-        <f t="shared" si="0"/>
-        <v>42.034682506824353</v>
-      </c>
-    </row>
-    <row r="39" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G39" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" s="17">
-        <f>H32</f>
-        <v>1790</v>
-      </c>
-      <c r="J39" s="18">
-        <v>3520</v>
-      </c>
-      <c r="T39" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="U39" s="15">
-        <f>2439.4</f>
-        <v>2439.4</v>
-      </c>
-      <c r="V39" s="15">
-        <v>34.403199999999998</v>
-      </c>
-      <c r="W39" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="X39" s="15">
-        <v>2450</v>
-      </c>
-      <c r="Y39" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G40" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H40" s="17">
-        <v>0</v>
-      </c>
-      <c r="J40" s="18">
-        <f>J33</f>
-        <v>8000</v>
-      </c>
-      <c r="T40" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="U40" s="15">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
-        <v>5.1595000000000004</v>
-      </c>
-      <c r="V40" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB40" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC40" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD40" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE40" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF40" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG40" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH40" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI40" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="AJ40" s="15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="41" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="AB41" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC41">
-        <f>AC35</f>
-        <v>2439.4</v>
-      </c>
-      <c r="AD41" t="str">
-        <f t="shared" ref="AD41:AH41" si="1">AD35</f>
-        <v>NA</v>
-      </c>
-      <c r="AE41">
-        <f t="shared" si="1"/>
-        <v>3758.6090581055701</v>
-      </c>
-      <c r="AF41" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
-      </c>
-      <c r="AG41">
-        <f t="shared" si="1"/>
-        <v>16.691730056956946</v>
-      </c>
-      <c r="AH41">
-        <f t="shared" si="1"/>
-        <v>42.034682506824353</v>
-      </c>
-    </row>
-    <row r="42" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G42" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J42" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="T42" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="U42" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="V42" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="W42" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="X42" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="Y42" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G43" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H43" s="17">
-        <f>H50</f>
-        <v>2439</v>
-      </c>
-      <c r="J43" s="18">
-        <v>0</v>
-      </c>
-      <c r="T43" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="U43" s="15">
-        <v>0</v>
-      </c>
-      <c r="V43" s="15">
-        <v>0</v>
-      </c>
-      <c r="W43" s="15">
-        <f>AVERAGE(2900,3100)</f>
-        <v>3000</v>
-      </c>
-      <c r="X43" s="15">
-        <v>398.15</v>
-      </c>
-      <c r="Y43" s="15">
+      <c r="Y43">
         <f>VLOOKUP($T43,MatExport[#All],7,FALSE)
 +VLOOKUP($T43,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T43,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>120</v>
       </c>
-      <c r="AB43" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AC43" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="AD43" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE43" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF43" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG43" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH43" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI43" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="AJ43" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="AK43" s="15" t="s">
-        <v>48</v>
+      <c r="AB43" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC43">
+        <f>AC39</f>
+        <v>2439.4</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE43">
+        <f>AE35*(($AC36-$AC35)/$AC$39)^3+AE36*(($AC37-$AC36)/$AC$39)^3+AE37*(($AC38-$AC36)/$AC$39)^3+AE38*(($AC39-$AC38)/$AC$39)^3</f>
+        <v>3758.6090581055701</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>182</v>
+      </c>
+      <c r="AG43">
+        <f>AG35*(($AC36-$AC35)/$AC$39)^3+AG36*(($AC37-$AC36)/$AC$39)^3+AG37*(($AC38-$AC36)/$AC$39)^3+AG38*(($AC39-$AC38)/$AC$39)^3</f>
+        <v>16.691730056956946</v>
+      </c>
+      <c r="AH43">
+        <f>AH35*(($AC36-$AC35)/$AC$39)^3+AH36*(($AC37-$AC36)/$AC$39)^3+AH37*(($AC38-$AC36)/$AC$39)^3+AH38*(($AC39-$AC38)/$AC$39)^3</f>
+        <v>42.034682506824353</v>
       </c>
     </row>
     <row r="44" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H44">
         <f>H51</f>
         <v>2339</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J44" s="15">
         <v>2900</v>
       </c>
-      <c r="T44" s="15" t="s">
+      <c r="T44" t="s">
         <v>89</v>
       </c>
       <c r="U44" s="1">
         <v>112.45399999999999</v>
       </c>
-      <c r="V44" s="15">
+      <c r="V44">
         <v>1.4930000000000001</v>
       </c>
-      <c r="W44" s="15">
+      <c r="W44">
         <f>VLOOKUP(T44,MatExport[],4,FALSE)</f>
         <v>3307.6</v>
       </c>
-      <c r="X44" s="15">
+      <c r="X44">
         <v>1099.75</v>
       </c>
-      <c r="Y44" s="15">
+      <c r="Y44">
         <f>VLOOKUP($T44,MatExport[#All],7,FALSE)
 +VLOOKUP($T44,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T44,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-      <c r="AB44" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC44" s="15">
-        <f>AC27</f>
-        <v>0</v>
-      </c>
-      <c r="AD44" s="15">
-        <f t="shared" ref="AD44:AI44" si="2">AD27</f>
-        <v>0</v>
-      </c>
-      <c r="AE44" s="15">
-        <f t="shared" si="2"/>
-        <v>3100</v>
-      </c>
-      <c r="AF44" s="15">
-        <f t="shared" si="2"/>
-        <v>398.15</v>
-      </c>
-      <c r="AG44" s="15">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="AH44" s="15">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="AI44" s="15">
-        <f t="shared" si="2"/>
-        <v>9.9999999999999992E+22</v>
-      </c>
     </row>
     <row r="45" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H45" s="17">
+      <c r="H45">
         <v>2070</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="15">
         <v>3280</v>
       </c>
-      <c r="T45" s="15" t="s">
+      <c r="T45" t="s">
         <v>85</v>
       </c>
-      <c r="U45" s="15">
+      <c r="U45">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,5,FALSE)</f>
         <v>2011.0545999999999</v>
       </c>
-      <c r="V45" s="15">
+      <c r="V45">
         <v>2.4287999999999998</v>
       </c>
-      <c r="W45" s="15">
+      <c r="W45">
         <f>VLOOKUP(T45,MatExport[],4,FALSE)</f>
         <v>7019</v>
       </c>
-      <c r="X45" s="15">
+      <c r="X45">
         <v>1800</v>
       </c>
-      <c r="Y45" s="15">
+      <c r="Y45">
         <f>VLOOKUP($T45,MatExport[#All],7,FALSE)
 +VLOOKUP($T45,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T45,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>-862.70086415590015</v>
       </c>
-      <c r="AB45" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC45" s="15">
-        <f t="shared" ref="AC45:AI48" si="3">AC28</f>
-        <v>112.45399999999999</v>
-      </c>
-      <c r="AD45" s="15">
-        <f t="shared" si="3"/>
-        <v>1.3422000000000001</v>
-      </c>
-      <c r="AE45" s="15">
-        <f t="shared" si="3"/>
-        <v>3307.6</v>
-      </c>
-      <c r="AF45" s="15">
-        <f t="shared" si="3"/>
-        <v>1099.75</v>
-      </c>
-      <c r="AG45" s="15">
-        <f t="shared" si="3"/>
-        <v>129.89999999999998</v>
-      </c>
-      <c r="AH45" s="15">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="AI45" s="15">
-        <f t="shared" si="3"/>
-        <v>1E+20</v>
+      <c r="AB45" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H46" s="17">
+      <c r="H46">
         <f>H53</f>
         <v>1790</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="15">
         <v>3390</v>
       </c>
-      <c r="T46" s="15" t="s">
+      <c r="T46" t="s">
         <v>55</v>
       </c>
-      <c r="U46" s="15">
+      <c r="U46">
         <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,4,FALSE)</f>
         <v>1342.6297999999999</v>
       </c>
-      <c r="V46" s="15">
+      <c r="V46">
         <v>21.718399999999999</v>
       </c>
-      <c r="W46" s="15">
+      <c r="W46">
         <f>VLOOKUP(T46,MatExport[],4,FALSE)</f>
         <v>7225</v>
       </c>
-      <c r="X46" s="15">
+      <c r="X46">
         <v>2450</v>
       </c>
-      <c r="Y46" s="15">
+      <c r="Y46">
         <f>VLOOKUP($T46,MatExport[#All],7,FALSE)
 +VLOOKUP($T46,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T46,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>127</v>
       </c>
-      <c r="AB46" s="15" t="s">
+      <c r="AB46" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC46">
+        <f>AC43</f>
+        <v>2439.4</v>
+      </c>
+      <c r="AD46" t="str">
+        <f t="shared" ref="AD46:AH46" si="0">AD43</f>
+        <v>NA</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" si="0"/>
+        <v>3758.6090581055701</v>
+      </c>
+      <c r="AF46" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="AG46">
+        <f t="shared" si="0"/>
+        <v>16.691730056956946</v>
+      </c>
+      <c r="AH46">
+        <f t="shared" si="0"/>
+        <v>42.034682506824353</v>
+      </c>
+    </row>
+    <row r="47" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G47" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="J47" s="15">
+        <f>J40</f>
+        <v>8000</v>
+      </c>
+      <c r="T47" t="s">
+        <v>180</v>
+      </c>
+      <c r="U47">
+        <f>2439.4</f>
+        <v>2439.4</v>
+      </c>
+      <c r="V47">
+        <v>34.403199999999998</v>
+      </c>
+      <c r="W47" t="s">
+        <v>182</v>
+      </c>
+      <c r="X47">
+        <v>2450</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="T48" t="s">
+        <v>178</v>
+      </c>
+      <c r="U48">
+        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
+        <v>5.1595000000000004</v>
+      </c>
+      <c r="V48" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB48" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G49" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I49" t="s">
+        <v>113</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC49">
+        <f>AC43</f>
+        <v>2439.4</v>
+      </c>
+      <c r="AD49" t="str">
+        <f t="shared" ref="AD49:AH49" si="1">AD43</f>
+        <v>NA</v>
+      </c>
+      <c r="AE49">
+        <f t="shared" si="1"/>
+        <v>3758.6090581055701</v>
+      </c>
+      <c r="AF49" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="AG49">
+        <f t="shared" si="1"/>
+        <v>16.691730056956946</v>
+      </c>
+      <c r="AH49">
+        <f t="shared" si="1"/>
+        <v>42.034682506824353</v>
+      </c>
+    </row>
+    <row r="50" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G50" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50">
+        <f>H36</f>
+        <v>2439</v>
+      </c>
+      <c r="J50" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G51" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H51">
+        <f>H37</f>
+        <v>2339</v>
+      </c>
+      <c r="J51" s="15">
+        <v>2900</v>
+      </c>
+      <c r="AB51" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G52" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H52">
+        <v>2040</v>
+      </c>
+      <c r="J52" s="15">
+        <v>3090</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC52">
+        <f>AC35</f>
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" ref="AD52:AI52" si="2">AD35</f>
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <f t="shared" si="2"/>
+        <v>3100</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="2"/>
+        <v>398.15</v>
+      </c>
+      <c r="AG52">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="AH52">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="AI52">
+        <f t="shared" si="2"/>
+        <v>9.9999999999999992E+22</v>
+      </c>
+    </row>
+    <row r="53" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G53" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H53">
+        <f>H39</f>
+        <v>1790</v>
+      </c>
+      <c r="J53" s="15">
+        <v>3250</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC53">
+        <f t="shared" ref="AC53:AI56" si="3">AC36</f>
+        <v>112.45399999999999</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="3"/>
+        <v>1.3422000000000001</v>
+      </c>
+      <c r="AE53">
+        <f t="shared" si="3"/>
+        <v>3307.6</v>
+      </c>
+      <c r="AF53">
+        <f t="shared" si="3"/>
+        <v>1099.75</v>
+      </c>
+      <c r="AG53">
+        <f t="shared" si="3"/>
+        <v>129.89999999999998</v>
+      </c>
+      <c r="AH53">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="AI53">
+        <f t="shared" si="3"/>
+        <v>1E+20</v>
+      </c>
+    </row>
+    <row r="54" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="G54" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="J54" s="15">
+        <f>J47</f>
+        <v>8000</v>
+      </c>
+      <c r="AB54" t="s">
         <v>85</v>
       </c>
-      <c r="AC46" s="15">
+      <c r="AC54">
         <f t="shared" si="3"/>
         <v>1326.0509999999999</v>
       </c>
-      <c r="AD46" s="15">
+      <c r="AD54">
         <f t="shared" si="3"/>
         <v>4.3647</v>
       </c>
-      <c r="AE46" s="15">
+      <c r="AE54">
         <f t="shared" si="3"/>
         <v>7019</v>
       </c>
-      <c r="AF46" s="15">
+      <c r="AF54">
         <f t="shared" si="3"/>
         <v>1800</v>
       </c>
-      <c r="AG46" s="15">
+      <c r="AG54">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AH46" s="15">
+      <c r="AH54">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="AI46" s="15">
+      <c r="AI54">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="G47" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H47" s="17">
-        <v>0</v>
-      </c>
-      <c r="J47" s="18">
-        <f>J40</f>
-        <v>8000</v>
-      </c>
-      <c r="T47" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="U47" s="15">
-        <f>2439.4</f>
-        <v>2439.4</v>
-      </c>
-      <c r="V47" s="15">
-        <v>34.403199999999998</v>
-      </c>
-      <c r="W47" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="X47" s="15">
-        <v>2450</v>
-      </c>
-      <c r="Y47" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB47" s="15" t="s">
+    <row r="55" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AB55" t="s">
         <v>55</v>
       </c>
-      <c r="AC47" s="15">
+      <c r="AC55">
         <f t="shared" si="3"/>
         <v>2011.5958000000001</v>
       </c>
-      <c r="AD47" s="15">
+      <c r="AD55">
         <f t="shared" si="3"/>
         <v>21.886399999999998</v>
       </c>
-      <c r="AE47" s="15">
+      <c r="AE55">
         <f t="shared" si="3"/>
         <v>7225</v>
       </c>
-      <c r="AF47" s="15">
+      <c r="AF55">
         <f t="shared" si="3"/>
         <v>2450</v>
       </c>
-      <c r="AG47" s="15">
+      <c r="AG55">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="AH47" s="15">
+      <c r="AH55">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="AI47" s="15">
+      <c r="AI55">
         <f t="shared" si="3"/>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="48" spans="7:37" x14ac:dyDescent="0.3">
-      <c r="T48" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="U48" s="15">
-        <f>VLOOKUP(_xlfn.CONCAT($L$31,$L$29),AS1Model2!$A$1:$L$17,6,FALSE)</f>
-        <v>5.1595000000000004</v>
-      </c>
-      <c r="V48" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB48" s="15" t="s">
+    <row r="56" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AB56" t="s">
         <v>180</v>
       </c>
-      <c r="AC48" s="15">
+      <c r="AC56">
         <f t="shared" si="3"/>
         <v>2439.4</v>
       </c>
-      <c r="AD48" s="15">
+      <c r="AD56">
         <f t="shared" si="3"/>
         <v>35.418999999999997</v>
       </c>
-      <c r="AE48" s="15" t="str">
+      <c r="AE56" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="AF48" s="15">
+      <c r="AF56">
         <f t="shared" si="3"/>
         <v>2450</v>
       </c>
-      <c r="AG48" s="15" t="str">
+      <c r="AG56" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="AH48" s="15" t="str">
+      <c r="AH56" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="AI48" s="15" t="str">
+      <c r="AI56" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="49" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G49" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="H49" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I49" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J49" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G50" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H50" s="17">
-        <f>H36</f>
-        <v>2439</v>
-      </c>
-      <c r="J50" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G51" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H51" s="17">
-        <f>H37</f>
-        <v>2339</v>
-      </c>
-      <c r="J51" s="18">
-        <v>2900</v>
-      </c>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="15"/>
-    </row>
-    <row r="52" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G52" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H52" s="17">
-        <v>2040</v>
-      </c>
-      <c r="J52" s="18">
-        <v>3090</v>
-      </c>
-    </row>
-    <row r="53" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G53" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H53" s="17">
-        <f>H39</f>
-        <v>1790</v>
-      </c>
-      <c r="J53" s="18">
-        <v>3250</v>
-      </c>
-    </row>
-    <row r="54" spans="7:30" x14ac:dyDescent="0.3">
-      <c r="G54" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H54" s="17">
-        <v>0</v>
-      </c>
-      <c r="J54" s="18">
-        <f>J47</f>
-        <v>8000</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" xr:uid="{1231B06C-7F06-44CD-B22C-5589D3ABEEC3}"/>
     <hyperlink ref="Z5" r:id="rId2" xr:uid="{7ED2418C-04A1-4B81-AAD6-9C03995326A4}"/>
     <hyperlink ref="AH5" r:id="rId3" xr:uid="{427C5272-4608-4461-9643-DA8CBB2537B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -11616,28 +11779,28 @@
       <c r="C90"/>
       <c r="E90"/>
       <c r="F90"/>
-      <c r="G90" s="10" t="s">
+      <c r="G90" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H90" s="10"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="10" t="s">
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="19"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="19"/>
+      <c r="M90" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="N90" s="10"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="10"/>
-      <c r="Q90" s="10"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="10" t="s">
+      <c r="N90" s="19"/>
+      <c r="O90" s="19"/>
+      <c r="P90" s="19"/>
+      <c r="Q90" s="19"/>
+      <c r="R90" s="19"/>
+      <c r="S90" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
-      <c r="V90" s="10"/>
+      <c r="T90" s="19"/>
+      <c r="U90" s="19"/>
+      <c r="V90" s="19"/>
       <c r="AD90"/>
       <c r="AG90"/>
     </row>

</xml_diff>

<commit_message>
added papers referenced from AS1, AS3 documentation and new papers in ref folder - added git debug commands with fix for large files handling
</commit_message>
<xml_diff>
--- a/MercuryModel.xlsx
+++ b/MercuryModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d679a80baeebce9/Documents/TU-Delft/AE4893 Physics of Planetary interiors/Assignment 3/PPI_AS3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71A0569-121E-4744-A1B5-18F9B6E22FF2}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA36723-1636-4CA8-AAF3-7264D3607B5D}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="2" r:id="rId1"/>
@@ -2400,8 +2400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB330E3-6480-4A3B-99B7-DBDC59EB106C}">
   <dimension ref="B2:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AJ5" sqref="AJ5"/>
+    <sheetView tabSelected="1" topLeftCell="T34" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="AM46" sqref="AM46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4544,6 +4544,9 @@
         <f>AH35*(($AC36-$AC35)/$AC$39)^3+AH36*(($AC37-$AC36)/$AC$39)^3+AH37*(($AC38-$AC36)/$AC$39)^3+AH38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>42.034682506824353</v>
       </c>
+      <c r="AI43" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="7:37" x14ac:dyDescent="0.3">
       <c r="G44" s="16" t="s">
@@ -5037,7 +5040,7 @@
         <v>2439.4</v>
       </c>
       <c r="AD56">
-        <f t="shared" si="3"/>
+        <f>AD39</f>
         <v>35.418999999999997</v>
       </c>
       <c r="AE56" t="str">
@@ -5771,8 +5774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:BI126"/>
   <sheetViews>
-    <sheetView topLeftCell="AY25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BI44" sqref="BI44"/>
+    <sheetView topLeftCell="AN2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BH37" sqref="BH37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated multi layer to sweep, updated other files
</commit_message>
<xml_diff>
--- a/MercuryModel.xlsx
+++ b/MercuryModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d679a80baeebce9/Documents/TU-Delft/AE4893 Physics of Planetary interiors/Assignment 3/PPI_AS3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA36723-1636-4CA8-AAF3-7264D3607B5D}"/>
+  <xr:revisionPtr revIDLastSave="573" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A274BE54-57B5-40C8-9C10-97A95EE9A3CB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="2" r:id="rId1"/>
@@ -65,6 +65,7 @@
     <author>tc={6EAC48A1-DE7E-44BF-A400-14FFD0D6EA9F}</author>
     <author>tc={AF0A2A2B-B375-4007-97E0-483D8B1CF039}</author>
     <author>tc={4BFCC566-92E8-4928-8748-52B17BD7C38D}</author>
+    <author>tc={68C06509-C383-4359-A953-88E2FF5BB3CE}</author>
     <author>tc={3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}</author>
     <author>tc={17382DD3-3CC6-4944-922C-7ED195CF53C3}</author>
     <author>tc={4805467D-952B-41B4-86D7-6B034FCD91D7}</author>
@@ -299,7 +300,15 @@
     =Dref, Te=NA</t>
       </text>
     </comment>
-    <comment ref="H38" authorId="22" shapeId="0" xr:uid="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
+    <comment ref="AH37" authorId="22" shapeId="0" xr:uid="{68C06509-C383-4359-A953-88E2FF5BB3CE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not corrected for sulfur content or pressure</t>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="23" shapeId="0" xr:uid="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -307,7 +316,7 @@
     Read from xs=0.05 on Fig3</t>
       </text>
     </comment>
-    <comment ref="J38" authorId="23" shapeId="0" xr:uid="{17382DD3-3CC6-4944-922C-7ED195CF53C3}">
+    <comment ref="J38" authorId="24" shapeId="0" xr:uid="{17382DD3-3CC6-4944-922C-7ED195CF53C3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -315,7 +324,7 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="T38" authorId="24" shapeId="0" xr:uid="{4805467D-952B-41B4-86D7-6B034FCD91D7}">
+    <comment ref="T38" authorId="25" shapeId="0" xr:uid="{4805467D-952B-41B4-86D7-6B034FCD91D7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +336,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="AB38" authorId="25" shapeId="0" xr:uid="{A4073D4E-E1DC-44B0-9181-10733F210188}">
+    <comment ref="AB38" authorId="26" shapeId="0" xr:uid="{A4073D4E-E1DC-44B0-9181-10733F210188}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -339,7 +348,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="J39" authorId="26" shapeId="0" xr:uid="{7C0DD50C-3623-48FA-84D7-1EF1D30CD771}">
+    <comment ref="J39" authorId="27" shapeId="0" xr:uid="{7C0DD50C-3623-48FA-84D7-1EF1D30CD771}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -347,7 +356,7 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="W43" authorId="27" shapeId="0" xr:uid="{46C7DEB7-FDA7-4ECC-B5F2-0B6956A449A2}">
+    <comment ref="W43" authorId="28" shapeId="0" xr:uid="{46C7DEB7-FDA7-4ECC-B5F2-0B6956A449A2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -355,7 +364,7 @@
     Free var</t>
       </text>
     </comment>
-    <comment ref="T44" authorId="28" shapeId="0" xr:uid="{7EC2AF2B-D535-47E2-9C1D-2D569E41F041}">
+    <comment ref="T44" authorId="29" shapeId="0" xr:uid="{7EC2AF2B-D535-47E2-9C1D-2D569E41F041}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -369,7 +378,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="U44" authorId="29" shapeId="0" xr:uid="{79ECA6B1-BECE-413E-9C45-4A24D2644F7E}">
+    <comment ref="U44" authorId="30" shapeId="0" xr:uid="{79ECA6B1-BECE-413E-9C45-4A24D2644F7E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -377,7 +386,7 @@
     =Dref, Te=Na</t>
       </text>
     </comment>
-    <comment ref="H45" authorId="30" shapeId="0" xr:uid="{568C4B86-2216-406C-86BF-93282A9B44DA}">
+    <comment ref="H45" authorId="31" shapeId="0" xr:uid="{568C4B86-2216-406C-86BF-93282A9B44DA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -385,7 +394,7 @@
     Read from xs=0.05 on Fig3</t>
       </text>
     </comment>
-    <comment ref="J45" authorId="31" shapeId="0" xr:uid="{E53C2281-5DE5-4BAE-9CA8-AA59645AF35A}">
+    <comment ref="J45" authorId="32" shapeId="0" xr:uid="{E53C2281-5DE5-4BAE-9CA8-AA59645AF35A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -393,7 +402,7 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="J46" authorId="32" shapeId="0" xr:uid="{F64A0414-C080-44D3-BE04-DD130B25B6AF}">
+    <comment ref="J46" authorId="33" shapeId="0" xr:uid="{F64A0414-C080-44D3-BE04-DD130B25B6AF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -401,7 +410,7 @@
     Read from Fig2</t>
       </text>
     </comment>
-    <comment ref="T46" authorId="33" shapeId="0" xr:uid="{7DCC7CBF-AB44-4661-B4E3-98FCB5363E48}">
+    <comment ref="T46" authorId="34" shapeId="0" xr:uid="{7DCC7CBF-AB44-4661-B4E3-98FCB5363E48}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -413,7 +422,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="H52" authorId="34" shapeId="0" xr:uid="{A1E3EE33-FD30-4342-A18D-A907A127862E}">
+    <comment ref="H52" authorId="35" shapeId="0" xr:uid="{A1E3EE33-FD30-4342-A18D-A907A127862E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -421,7 +430,7 @@
     Read from xs=0.05 on Fig3</t>
       </text>
     </comment>
-    <comment ref="J53" authorId="35" shapeId="0" xr:uid="{AAD794F5-F5C5-42BE-A4C0-4E15D7C71744}">
+    <comment ref="J53" authorId="36" shapeId="0" xr:uid="{AAD794F5-F5C5-42BE-A4C0-4E15D7C71744}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -496,7 +505,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="246">
   <si>
     <t>T_0</t>
   </si>
@@ -1216,6 +1225,24 @@
   </si>
   <si>
     <t>S1, fluid</t>
+  </si>
+  <si>
+    <t>depth [km]</t>
+  </si>
+  <si>
+    <t>mu0</t>
+  </si>
+  <si>
+    <t>eta0</t>
+  </si>
+  <si>
+    <t>rho0</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>Ks0</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1374,6 +1401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2313,6 +2341,9 @@
   <threadedComment ref="AC36" dT="2024-06-27T12:12:15.58" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{4BFCC566-92E8-4928-8748-52B17BD7C38D}">
     <text>=Dref, Te=NA</text>
   </threadedComment>
+  <threadedComment ref="AH37" dT="2024-06-28T12:23:36.17" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{68C06509-C383-4359-A953-88E2FF5BB3CE}">
+    <text>Not corrected for sulfur content or pressure</text>
+  </threadedComment>
   <threadedComment ref="H38" dT="2024-04-30T15:19:22.86" personId="{F3D40453-295F-4F96-A9FE-C7BF675D9F13}" id="{3F4AEE8F-75BB-40DE-B1BF-D0685A1002F9}">
     <text>Read from xs=0.05 on Fig3</text>
   </threadedComment>
@@ -2400,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB330E3-6480-4A3B-99B7-DBDC59EB106C}">
   <dimension ref="B2:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T34" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AM46" sqref="AM46"/>
+    <sheetView tabSelected="1" topLeftCell="Z36" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4017,7 +4048,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G33" s="16" t="s">
         <v>119</v>
       </c>
@@ -4028,8 +4059,23 @@
         <f>J26</f>
         <v>8000</v>
       </c>
-    </row>
-    <row r="34" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AD33" t="s">
+        <v>244</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>245</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>241</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="7:38" x14ac:dyDescent="0.3">
       <c r="L34" s="16" t="s">
         <v>178</v>
       </c>
@@ -4062,28 +4108,31 @@
         <v>207</v>
       </c>
       <c r="AC34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD34" t="s">
         <v>191</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AE34" t="s">
         <v>113</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AF34" t="s">
         <v>92</v>
       </c>
-      <c r="AF34" t="s">
+      <c r="AG34" t="s">
         <v>192</v>
       </c>
-      <c r="AG34" t="s">
+      <c r="AH34" t="s">
         <v>208</v>
       </c>
-      <c r="AH34" t="s">
+      <c r="AI34" t="s">
         <v>209</v>
       </c>
-      <c r="AI34" t="s">
+      <c r="AJ34" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G35" s="14" t="s">
         <v>125</v>
       </c>
@@ -4125,30 +4174,33 @@
         <v>0</v>
       </c>
       <c r="AD35">
-        <v>0</v>
-      </c>
-      <c r="AE35" s="5">
+        <f>$AC$39-AC35</f>
+        <v>2439.4</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="5">
         <v>3100</v>
       </c>
-      <c r="AF35">
+      <c r="AG35">
         <v>398.15</v>
       </c>
-      <c r="AG35">
+      <c r="AH35">
         <f>VLOOKUP($T19,MatExport[#All],7,FALSE)
 +VLOOKUP($T19,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T19,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>120</v>
       </c>
-      <c r="AH35" s="5">
-        <f>$AD$19</f>
-        <v>70</v>
-      </c>
-      <c r="AI35">
+      <c r="AI35" s="5">
+        <v>55</v>
+      </c>
+      <c r="AJ35">
         <f>10^23</f>
         <v>9.9999999999999992E+22</v>
       </c>
     </row>
-    <row r="36" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G36" s="16" t="s">
         <v>114</v>
       </c>
@@ -4188,31 +4240,35 @@
         <v>112.45399999999999</v>
       </c>
       <c r="AD36">
+        <f t="shared" ref="AD36:AD39" si="0">$AC$39-AC36</f>
+        <v>2326.9459999999999</v>
+      </c>
+      <c r="AE36">
         <v>1.3422000000000001</v>
       </c>
-      <c r="AE36">
+      <c r="AF36">
         <f>VLOOKUP(AB36,MatExport[],4,FALSE)</f>
         <v>3307.6</v>
       </c>
-      <c r="AF36">
+      <c r="AG36">
         <v>1099.75</v>
       </c>
-      <c r="AG36">
+      <c r="AH36">
         <f>VLOOKUP($T20,MatExport[#All],7,FALSE)
 +VLOOKUP($T20,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T20,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-      <c r="AH36" s="5">
-        <f>$AD$19</f>
-        <v>70</v>
-      </c>
-      <c r="AI36">
-        <f>AD20</f>
-        <v>1E+20</v>
-      </c>
-    </row>
-    <row r="37" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AI36" s="5">
+        <f>65</f>
+        <v>65</v>
+      </c>
+      <c r="AJ36" s="7">
+        <f>10^11</f>
+        <v>100000000000</v>
+      </c>
+    </row>
+    <row r="37" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G37" s="16" t="s">
         <v>116</v>
       </c>
@@ -4253,27 +4309,31 @@
         <v>1326.0509999999999</v>
       </c>
       <c r="AD37">
+        <f t="shared" si="0"/>
+        <v>1113.3490000000002</v>
+      </c>
+      <c r="AE37">
         <v>4.3647</v>
       </c>
-      <c r="AE37">
+      <c r="AF37">
         <f>VLOOKUP(AB37,MatExport[],4,FALSE)</f>
         <v>7019</v>
       </c>
-      <c r="AF37">
+      <c r="AG37">
         <v>1800</v>
       </c>
-      <c r="AG37">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="5">
-        <f>$AD$19</f>
-        <v>70</v>
-      </c>
-      <c r="AI37" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AH37" s="4">
+        <f>VLOOKUP($T21,MatExport[#All],7,FALSE)</f>
+        <v>85.9</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G38" s="16" t="s">
         <v>67</v>
       </c>
@@ -4313,31 +4373,34 @@
         <v>2011.5958000000001</v>
       </c>
       <c r="AD38">
+        <f t="shared" si="0"/>
+        <v>427.80420000000004</v>
+      </c>
+      <c r="AE38">
         <v>21.886399999999998</v>
       </c>
-      <c r="AE38">
+      <c r="AF38">
         <f>VLOOKUP(AB38,MatExport[],4,FALSE)</f>
         <v>7225</v>
       </c>
-      <c r="AF38">
+      <c r="AG38">
         <v>2450</v>
       </c>
-      <c r="AG38">
+      <c r="AH38">
         <f>VLOOKUP($T22,MatExport[#All],7,FALSE)
 +VLOOKUP($T22,MatExport[#All],5,FALSE)*($M$34/100)
 +VLOOKUP($T22,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>127</v>
       </c>
-      <c r="AH38" s="5">
-        <f>$AD$19</f>
-        <v>70</v>
-      </c>
       <c r="AI38">
+        <v>100</v>
+      </c>
+      <c r="AJ38">
         <f>10^20</f>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="39" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G39" s="16" t="s">
         <v>122</v>
       </c>
@@ -4375,16 +4438,17 @@
         <v>2439.4</v>
       </c>
       <c r="AD39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE39">
         <v>35.418999999999997</v>
       </c>
-      <c r="AE39" t="s">
+      <c r="AF39" t="s">
         <v>182</v>
       </c>
-      <c r="AF39">
+      <c r="AG39">
         <v>2450</v>
-      </c>
-      <c r="AG39" t="s">
-        <v>182</v>
       </c>
       <c r="AH39" t="s">
         <v>182</v>
@@ -4392,8 +4456,11 @@
       <c r="AI39" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="40" spans="7:37" x14ac:dyDescent="0.3">
+      <c r="AJ39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G40" s="16" t="s">
         <v>119</v>
       </c>
@@ -4420,11 +4487,11 @@
       <c r="AC40">
         <v>5.2923999999999998</v>
       </c>
-      <c r="AD40" t="s">
+      <c r="AE40" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G42" s="14" t="s">
         <v>126</v>
       </c>
@@ -4459,34 +4526,37 @@
         <v>227</v>
       </c>
       <c r="AC42" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD42" t="s">
         <v>191</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>113</v>
       </c>
-      <c r="AE42" t="s">
+      <c r="AF42" t="s">
         <v>92</v>
       </c>
-      <c r="AF42" t="s">
+      <c r="AG42" t="s">
         <v>192</v>
       </c>
-      <c r="AG42" t="s">
+      <c r="AH42" t="s">
         <v>208</v>
       </c>
-      <c r="AH42" t="s">
+      <c r="AI42" t="s">
         <v>209</v>
       </c>
-      <c r="AI42" t="s">
+      <c r="AJ42" t="s">
         <v>193</v>
       </c>
-      <c r="AJ42" t="s">
+      <c r="AK42" t="s">
         <v>226</v>
       </c>
-      <c r="AK42" t="s">
+      <c r="AL42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G43" s="16" t="s">
         <v>114</v>
       </c>
@@ -4526,29 +4596,34 @@
         <f>AC39</f>
         <v>2439.4</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AD43">
+        <f t="shared" ref="AD43" si="1">$AC$39-AC43</f>
+        <v>0</v>
+      </c>
+      <c r="AE43" t="s">
         <v>182</v>
       </c>
-      <c r="AE43">
-        <f>AE35*(($AC36-$AC35)/$AC$39)^3+AE36*(($AC37-$AC36)/$AC$39)^3+AE37*(($AC38-$AC36)/$AC$39)^3+AE38*(($AC39-$AC38)/$AC$39)^3</f>
+      <c r="AF43" s="20">
+        <f>AF35*(($AC36-$AC35)/$AC$39)^3+AF36*(($AC37-$AC36)/$AC$39)^3+AF37*(($AC38-$AC36)/$AC$39)^3+AF38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>3758.6090581055701</v>
       </c>
-      <c r="AF43" t="s">
+      <c r="AG43" t="s">
         <v>182</v>
       </c>
-      <c r="AG43">
-        <f>AG35*(($AC36-$AC35)/$AC$39)^3+AG36*(($AC37-$AC36)/$AC$39)^3+AG37*(($AC38-$AC36)/$AC$39)^3+AG38*(($AC39-$AC38)/$AC$39)^3</f>
-        <v>16.691730056956946</v>
-      </c>
-      <c r="AH43">
+      <c r="AH43" s="20">
         <f>AH35*(($AC36-$AC35)/$AC$39)^3+AH36*(($AC37-$AC36)/$AC$39)^3+AH37*(($AC38-$AC36)/$AC$39)^3+AH38*(($AC39-$AC38)/$AC$39)^3</f>
-        <v>42.034682506824353</v>
-      </c>
-      <c r="AI43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="7:37" x14ac:dyDescent="0.3">
+        <v>57.225433283399752</v>
+      </c>
+      <c r="AI43" s="20">
+        <f>AI35*(($AC36-$AC35)/$AC$39)^3+AI36*(($AC37-$AC36)/$AC$39)^3+AI37*(($AC38-$AC36)/$AC$39)^3+AI38*(($AC39-$AC38)/$AC$39)^3</f>
+        <v>8.5484015741282242</v>
+      </c>
+      <c r="AJ43">
+        <f>AJ35*(($AC36-$AC35)/$AC$39)^3+AJ36*(($AC37-$AC36)/$AC$39)^3+AJ37*(($AC38-$AC36)/$AC$39)^3+AJ38*(($AC39-$AC38)/$AC$39)^3</f>
+        <v>1.0335975654962989E+19</v>
+      </c>
+    </row>
+    <row r="44" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G44" s="16" t="s">
         <v>116</v>
       </c>
@@ -4582,7 +4657,7 @@
         <v>129.89999999999998</v>
       </c>
     </row>
-    <row r="45" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G45" s="16" t="s">
         <v>67</v>
       </c>
@@ -4619,31 +4694,34 @@
         <v>228</v>
       </c>
       <c r="AC45" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD45" t="s">
         <v>191</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AE45" t="s">
         <v>113</v>
       </c>
-      <c r="AE45" t="s">
+      <c r="AF45" t="s">
         <v>92</v>
       </c>
-      <c r="AF45" t="s">
+      <c r="AG45" t="s">
         <v>192</v>
       </c>
-      <c r="AG45" t="s">
+      <c r="AH45" t="s">
         <v>208</v>
       </c>
-      <c r="AH45" t="s">
+      <c r="AI45" t="s">
         <v>209</v>
       </c>
-      <c r="AI45" t="s">
+      <c r="AJ45" t="s">
         <v>193</v>
       </c>
-      <c r="AJ45" t="s">
+      <c r="AK45" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G46" s="16" t="s">
         <v>122</v>
       </c>
@@ -4684,28 +4762,36 @@
         <f>AC43</f>
         <v>2439.4</v>
       </c>
-      <c r="AD46" t="str">
-        <f t="shared" ref="AD46:AH46" si="0">AD43</f>
+      <c r="AD46">
+        <f t="shared" ref="AD46" si="2">$AC$39-AC46</f>
+        <v>0</v>
+      </c>
+      <c r="AE46" t="str">
+        <f t="shared" ref="AE46:AJ46" si="3">AE43</f>
         <v>NA</v>
       </c>
-      <c r="AE46">
-        <f t="shared" si="0"/>
+      <c r="AF46">
+        <f t="shared" si="3"/>
         <v>3758.6090581055701</v>
       </c>
-      <c r="AF46" t="str">
-        <f t="shared" si="0"/>
+      <c r="AG46" t="str">
+        <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="AG46">
-        <f t="shared" si="0"/>
-        <v>16.691730056956946</v>
-      </c>
       <c r="AH46">
-        <f t="shared" si="0"/>
-        <v>42.034682506824353</v>
-      </c>
-    </row>
-    <row r="47" spans="7:37" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>57.225433283399752</v>
+      </c>
+      <c r="AI46">
+        <f t="shared" si="3"/>
+        <v>8.5484015741282242</v>
+      </c>
+      <c r="AJ46">
+        <f t="shared" si="3"/>
+        <v>1.0335975654962989E+19</v>
+      </c>
+    </row>
+    <row r="47" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G47" s="16" t="s">
         <v>119</v>
       </c>
@@ -4736,7 +4822,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:38" x14ac:dyDescent="0.3">
       <c r="T48" t="s">
         <v>178</v>
       </c>
@@ -4751,31 +4837,34 @@
         <v>229</v>
       </c>
       <c r="AC48" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD48" t="s">
         <v>191</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AE48" t="s">
         <v>113</v>
       </c>
-      <c r="AE48" t="s">
+      <c r="AF48" t="s">
         <v>92</v>
       </c>
-      <c r="AF48" t="s">
+      <c r="AG48" t="s">
         <v>192</v>
       </c>
-      <c r="AG48" t="s">
+      <c r="AH48" t="s">
         <v>208</v>
       </c>
-      <c r="AH48" t="s">
+      <c r="AI48" t="s">
         <v>209</v>
       </c>
-      <c r="AI48" t="s">
+      <c r="AJ48" t="s">
         <v>193</v>
       </c>
-      <c r="AJ48" t="s">
+      <c r="AK48" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G49" s="14" t="s">
         <v>127</v>
       </c>
@@ -4795,28 +4884,32 @@
         <f>AC43</f>
         <v>2439.4</v>
       </c>
-      <c r="AD49" t="str">
-        <f t="shared" ref="AD49:AH49" si="1">AD43</f>
+      <c r="AD49">
+        <f t="shared" ref="AD49" si="4">$AC$39-AC49</f>
+        <v>0</v>
+      </c>
+      <c r="AE49" t="str">
+        <f t="shared" ref="AE49:AI49" si="5">AE43</f>
         <v>NA</v>
       </c>
-      <c r="AE49">
-        <f t="shared" si="1"/>
+      <c r="AF49">
+        <f t="shared" si="5"/>
         <v>3758.6090581055701</v>
       </c>
-      <c r="AF49" t="str">
-        <f t="shared" si="1"/>
+      <c r="AG49" t="str">
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="AG49">
-        <f t="shared" si="1"/>
-        <v>16.691730056956946</v>
-      </c>
       <c r="AH49">
-        <f t="shared" si="1"/>
-        <v>42.034682506824353</v>
-      </c>
-    </row>
-    <row r="50" spans="7:37" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>57.225433283399752</v>
+      </c>
+      <c r="AI49">
+        <f t="shared" si="5"/>
+        <v>8.5484015741282242</v>
+      </c>
+    </row>
+    <row r="50" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G50" s="16" t="s">
         <v>114</v>
       </c>
@@ -4828,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G51" s="16" t="s">
         <v>116</v>
       </c>
@@ -4843,34 +4936,37 @@
         <v>225</v>
       </c>
       <c r="AC51" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD51" t="s">
         <v>191</v>
       </c>
-      <c r="AD51" t="s">
+      <c r="AE51" t="s">
         <v>113</v>
       </c>
-      <c r="AE51" t="s">
+      <c r="AF51" t="s">
         <v>92</v>
       </c>
-      <c r="AF51" t="s">
+      <c r="AG51" t="s">
         <v>192</v>
       </c>
-      <c r="AG51" t="s">
+      <c r="AH51" t="s">
         <v>208</v>
       </c>
-      <c r="AH51" t="s">
+      <c r="AI51" t="s">
         <v>209</v>
       </c>
-      <c r="AI51" t="s">
+      <c r="AJ51" t="s">
         <v>193</v>
       </c>
-      <c r="AJ51" t="s">
+      <c r="AK51" t="s">
         <v>226</v>
       </c>
-      <c r="AK51" t="s">
+      <c r="AL51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G52" s="16" t="s">
         <v>67</v>
       </c>
@@ -4888,31 +4984,35 @@
         <v>0</v>
       </c>
       <c r="AD52">
-        <f t="shared" ref="AD52:AI52" si="2">AD35</f>
-        <v>0</v>
+        <f t="shared" ref="AD52" si="6">$AC$39-AC52</f>
+        <v>2439.4</v>
       </c>
       <c r="AE52">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AE52:AJ52" si="7">AE35</f>
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="7"/>
         <v>3100</v>
       </c>
-      <c r="AF52">
-        <f t="shared" si="2"/>
+      <c r="AG52">
+        <f t="shared" si="7"/>
         <v>398.15</v>
       </c>
-      <c r="AG52">
-        <f t="shared" si="2"/>
+      <c r="AH52">
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
-      <c r="AH52">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
       <c r="AI52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="AJ52">
+        <f t="shared" si="7"/>
         <v>9.9999999999999992E+22</v>
       </c>
     </row>
-    <row r="53" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G53" s="16" t="s">
         <v>122</v>
       </c>
@@ -4927,35 +5027,35 @@
         <v>89</v>
       </c>
       <c r="AC53">
-        <f t="shared" ref="AC53:AI56" si="3">AC36</f>
+        <f t="shared" ref="AC53:AC56" si="8">AC36</f>
         <v>112.45399999999999</v>
       </c>
-      <c r="AD53">
-        <f t="shared" si="3"/>
+      <c r="AE53">
+        <f t="shared" ref="AE53:AJ56" si="9">AE36</f>
         <v>1.3422000000000001</v>
       </c>
-      <c r="AE53">
-        <f t="shared" si="3"/>
+      <c r="AF53">
+        <f t="shared" si="9"/>
         <v>3307.6</v>
       </c>
-      <c r="AF53">
-        <f t="shared" si="3"/>
+      <c r="AG53">
+        <f t="shared" si="9"/>
         <v>1099.75</v>
       </c>
-      <c r="AG53">
-        <f t="shared" si="3"/>
+      <c r="AH53">
+        <f t="shared" si="9"/>
         <v>129.89999999999998</v>
       </c>
-      <c r="AH53">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
       <c r="AI53">
-        <f t="shared" si="3"/>
-        <v>1E+20</v>
-      </c>
-    </row>
-    <row r="54" spans="7:37" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="AJ53">
+        <f t="shared" si="9"/>
+        <v>100000000000</v>
+      </c>
+    </row>
+    <row r="54" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G54" s="16" t="s">
         <v>119</v>
       </c>
@@ -4970,97 +5070,97 @@
         <v>85</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1326.0509999999999</v>
       </c>
-      <c r="AD54">
-        <f t="shared" si="3"/>
+      <c r="AE54">
+        <f t="shared" si="9"/>
         <v>4.3647</v>
       </c>
-      <c r="AE54">
-        <f t="shared" si="3"/>
+      <c r="AF54">
+        <f t="shared" si="9"/>
         <v>7019</v>
       </c>
-      <c r="AF54">
-        <f t="shared" si="3"/>
+      <c r="AG54">
+        <f t="shared" si="9"/>
         <v>1800</v>
       </c>
-      <c r="AG54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="AH54">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f t="shared" si="9"/>
+        <v>85.9</v>
       </c>
       <c r="AI54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="7:37" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AJ54">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="7:38" x14ac:dyDescent="0.3">
       <c r="AB55" t="s">
         <v>55</v>
       </c>
       <c r="AC55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2011.5958000000001</v>
       </c>
-      <c r="AD55">
-        <f t="shared" si="3"/>
+      <c r="AE55">
+        <f t="shared" si="9"/>
         <v>21.886399999999998</v>
       </c>
-      <c r="AE55">
-        <f t="shared" si="3"/>
+      <c r="AF55">
+        <f t="shared" si="9"/>
         <v>7225</v>
       </c>
-      <c r="AF55">
-        <f t="shared" si="3"/>
+      <c r="AG55">
+        <f t="shared" si="9"/>
         <v>2450</v>
       </c>
-      <c r="AG55">
-        <f t="shared" si="3"/>
+      <c r="AH55">
+        <f t="shared" si="9"/>
         <v>127</v>
       </c>
-      <c r="AH55">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
       <c r="AI55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AJ55">
+        <f t="shared" si="9"/>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="56" spans="7:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:38" x14ac:dyDescent="0.3">
       <c r="AB56" t="s">
         <v>180</v>
       </c>
       <c r="AC56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2439.4</v>
       </c>
-      <c r="AD56">
-        <f>AD39</f>
+      <c r="AE56">
+        <f t="shared" si="9"/>
         <v>35.418999999999997</v>
       </c>
-      <c r="AE56" t="str">
-        <f t="shared" si="3"/>
+      <c r="AF56" t="str">
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
-      <c r="AF56">
-        <f t="shared" si="3"/>
+      <c r="AG56">
+        <f t="shared" si="9"/>
         <v>2450</v>
       </c>
-      <c r="AG56" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH56" t="str">
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
-      <c r="AH56" t="str">
-        <f t="shared" si="3"/>
+      <c r="AI56" t="str">
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
-      <c r="AI56" t="str">
-        <f t="shared" si="3"/>
+      <c r="AJ56" t="str">
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pushed forgotten files, added results h2,k2 in excel
</commit_message>
<xml_diff>
--- a/MercuryModel.xlsx
+++ b/MercuryModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d679a80baeebce9/Documents/TU-Delft/AE4893 Physics of Planetary interiors/Assignment 3/PPI_AS3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="573" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A274BE54-57B5-40C8-9C10-97A95EE9A3CB}"/>
+  <xr:revisionPtr revIDLastSave="606" documentId="11_F25DC773A252ABDACC104884E99D47E45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93700BB1-B898-4C16-B608-575BBEF5012D}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="254">
   <si>
     <t>T_0</t>
   </si>
@@ -1243,6 +1243,30 @@
   </si>
   <si>
     <t>Ks0</t>
+  </si>
+  <si>
+    <t>Re(h)</t>
+  </si>
+  <si>
+    <t>Im(h)</t>
+  </si>
+  <si>
+    <t>Re(k)</t>
+  </si>
+  <si>
+    <t>Im(k)</t>
+  </si>
+  <si>
+    <t>elastic</t>
+  </si>
+  <si>
+    <t>visco-elastic</t>
+  </si>
+  <si>
+    <t>ideal fluid</t>
+  </si>
+  <si>
+    <t>Mref</t>
   </si>
 </sst>
 </file>
@@ -1398,10 +1422,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2429,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB330E3-6480-4A3B-99B7-DBDC59EB106C}">
-  <dimension ref="B2:AO56"/>
+  <dimension ref="B2:AT56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z36" zoomScale="87" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+    <sheetView tabSelected="1" topLeftCell="AK29" zoomScale="85" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="AQ34" sqref="AQ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4048,7 +4072,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G33" s="16" t="s">
         <v>119</v>
       </c>
@@ -4074,8 +4098,20 @@
       <c r="AJ33" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="34" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AQ33" t="s">
+        <v>246</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>248</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="7:46" x14ac:dyDescent="0.3">
       <c r="L34" s="16" t="s">
         <v>178</v>
       </c>
@@ -4131,8 +4167,27 @@
       <c r="AJ34" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="35" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AP34" t="s">
+        <v>253</v>
+      </c>
+      <c r="AQ34">
+        <f>AK34</f>
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <f t="shared" ref="AR34" si="0">AL34</f>
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <f t="shared" ref="AS34" si="1">AM34</f>
+        <v>0</v>
+      </c>
+      <c r="AT34">
+        <f t="shared" ref="AT34" si="2">AN34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G35" s="14" t="s">
         <v>125</v>
       </c>
@@ -4200,7 +4255,7 @@
         <v>9.9999999999999992E+22</v>
       </c>
     </row>
-    <row r="36" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G36" s="16" t="s">
         <v>114</v>
       </c>
@@ -4240,7 +4295,7 @@
         <v>112.45399999999999</v>
       </c>
       <c r="AD36">
-        <f t="shared" ref="AD36:AD39" si="0">$AC$39-AC36</f>
+        <f t="shared" ref="AD36:AD39" si="3">$AC$39-AC36</f>
         <v>2326.9459999999999</v>
       </c>
       <c r="AE36">
@@ -4268,7 +4323,7 @@
         <v>100000000000</v>
       </c>
     </row>
-    <row r="37" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G37" s="16" t="s">
         <v>116</v>
       </c>
@@ -4309,7 +4364,7 @@
         <v>1326.0509999999999</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1113.3490000000002</v>
       </c>
       <c r="AE37">
@@ -4333,7 +4388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G38" s="16" t="s">
         <v>67</v>
       </c>
@@ -4373,7 +4428,7 @@
         <v>2011.5958000000001</v>
       </c>
       <c r="AD38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>427.80420000000004</v>
       </c>
       <c r="AE38">
@@ -4400,7 +4455,7 @@
         <v>1E+20</v>
       </c>
     </row>
-    <row r="39" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G39" s="16" t="s">
         <v>122</v>
       </c>
@@ -4438,7 +4493,7 @@
         <v>2439.4</v>
       </c>
       <c r="AD39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE39">
@@ -4460,7 +4515,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G40" s="16" t="s">
         <v>119</v>
       </c>
@@ -4491,7 +4546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G42" s="14" t="s">
         <v>126</v>
       </c>
@@ -4550,13 +4605,31 @@
         <v>193</v>
       </c>
       <c r="AK42" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="AL42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="7:38" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="AM42" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>249</v>
+      </c>
+      <c r="AQ42" t="s">
+        <v>246</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>247</v>
+      </c>
+      <c r="AS42" t="s">
+        <v>248</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G43" s="16" t="s">
         <v>114</v>
       </c>
@@ -4597,24 +4670,24 @@
         <v>2439.4</v>
       </c>
       <c r="AD43">
-        <f t="shared" ref="AD43" si="1">$AC$39-AC43</f>
+        <f t="shared" ref="AD43" si="4">$AC$39-AC43</f>
         <v>0</v>
       </c>
       <c r="AE43" t="s">
         <v>182</v>
       </c>
-      <c r="AF43" s="20">
+      <c r="AF43" s="19">
         <f>AF35*(($AC36-$AC35)/$AC$39)^3+AF36*(($AC37-$AC36)/$AC$39)^3+AF37*(($AC38-$AC36)/$AC$39)^3+AF38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>3758.6090581055701</v>
       </c>
       <c r="AG43" t="s">
         <v>182</v>
       </c>
-      <c r="AH43" s="20">
+      <c r="AH43" s="19">
         <f>AH35*(($AC36-$AC35)/$AC$39)^3+AH36*(($AC37-$AC36)/$AC$39)^3+AH37*(($AC38-$AC36)/$AC$39)^3+AH38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>57.225433283399752</v>
       </c>
-      <c r="AI43" s="20">
+      <c r="AI43" s="19">
         <f>AI35*(($AC36-$AC35)/$AC$39)^3+AI36*(($AC37-$AC36)/$AC$39)^3+AI37*(($AC38-$AC36)/$AC$39)^3+AI38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>8.5484015741282242</v>
       </c>
@@ -4622,8 +4695,39 @@
         <f>AJ35*(($AC36-$AC35)/$AC$39)^3+AJ36*(($AC37-$AC36)/$AC$39)^3+AJ37*(($AC38-$AC36)/$AC$39)^3+AJ38*(($AC39-$AC38)/$AC$39)^3</f>
         <v>1.0335975654962989E+19</v>
       </c>
-    </row>
-    <row r="44" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AK43">
+        <v>0.5726</v>
+      </c>
+      <c r="AL43">
+        <v>0</v>
+      </c>
+      <c r="AM43">
+        <v>0.3377</v>
+      </c>
+      <c r="AN43">
+        <v>0</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>250</v>
+      </c>
+      <c r="AQ43">
+        <f>AK43</f>
+        <v>0.5726</v>
+      </c>
+      <c r="AR43">
+        <f t="shared" ref="AR43:AT43" si="5">AL43</f>
+        <v>0</v>
+      </c>
+      <c r="AS43">
+        <f t="shared" si="5"/>
+        <v>0.3377</v>
+      </c>
+      <c r="AT43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G44" s="16" t="s">
         <v>116</v>
       </c>
@@ -4656,8 +4760,27 @@
 +VLOOKUP($T44,MatExport[#All],6,FALSE)*($M$34/100)^2</f>
         <v>129.89999999999998</v>
       </c>
-    </row>
-    <row r="45" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AP44" t="s">
+        <v>251</v>
+      </c>
+      <c r="AQ44">
+        <f>AK46</f>
+        <v>-1.9027000000000001</v>
+      </c>
+      <c r="AR44">
+        <f t="shared" ref="AR44:AT44" si="6">AL46</f>
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="AS44">
+        <f t="shared" si="6"/>
+        <v>-0.99619999999999997</v>
+      </c>
+      <c r="AT44">
+        <f t="shared" si="6"/>
+        <v>1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G45" s="16" t="s">
         <v>67</v>
       </c>
@@ -4718,10 +4841,38 @@
         <v>193</v>
       </c>
       <c r="AK45" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="46" spans="7:38" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>247</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>249</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>252</v>
+      </c>
+      <c r="AQ45">
+        <f>AK49</f>
+        <v>-0.38240000000000002</v>
+      </c>
+      <c r="AR45">
+        <f t="shared" ref="AR45:AT45" si="7">AL49</f>
+        <v>0.51</v>
+      </c>
+      <c r="AS45">
+        <f t="shared" si="7"/>
+        <v>-0.99880000000000002</v>
+      </c>
+      <c r="AT45">
+        <f t="shared" si="7"/>
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G46" s="16" t="s">
         <v>122</v>
       </c>
@@ -4763,35 +4914,47 @@
         <v>2439.4</v>
       </c>
       <c r="AD46">
-        <f t="shared" ref="AD46" si="2">$AC$39-AC46</f>
+        <f t="shared" ref="AD46" si="8">$AC$39-AC46</f>
         <v>0</v>
       </c>
       <c r="AE46" t="str">
-        <f t="shared" ref="AE46:AJ46" si="3">AE43</f>
+        <f t="shared" ref="AE46:AJ46" si="9">AE43</f>
         <v>NA</v>
       </c>
       <c r="AF46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3758.6090581055701</v>
       </c>
       <c r="AG46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="AH46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>57.225433283399752</v>
       </c>
       <c r="AI46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.5484015741282242</v>
       </c>
       <c r="AJ46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0335975654962989E+19</v>
       </c>
-    </row>
-    <row r="47" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AK46" s="13">
+        <v>-1.9027000000000001</v>
+      </c>
+      <c r="AL46" s="13">
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="AM46">
+        <v>-0.99619999999999997</v>
+      </c>
+      <c r="AN46">
+        <v>1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="7:46" x14ac:dyDescent="0.3">
       <c r="G47" s="16" t="s">
         <v>119</v>
       </c>
@@ -4822,7 +4985,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:46" x14ac:dyDescent="0.3">
       <c r="T48" t="s">
         <v>178</v>
       </c>
@@ -4861,10 +5024,19 @@
         <v>193</v>
       </c>
       <c r="AK48" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="7:38" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>247</v>
+      </c>
+      <c r="AM48" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN48" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G49" s="14" t="s">
         <v>127</v>
       </c>
@@ -4885,31 +5057,43 @@
         <v>2439.4</v>
       </c>
       <c r="AD49">
-        <f t="shared" ref="AD49" si="4">$AC$39-AC49</f>
+        <f t="shared" ref="AD49" si="10">$AC$39-AC49</f>
         <v>0</v>
       </c>
       <c r="AE49" t="str">
-        <f t="shared" ref="AE49:AI49" si="5">AE43</f>
+        <f t="shared" ref="AE49:AI49" si="11">AE43</f>
         <v>NA</v>
       </c>
       <c r="AF49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>3758.6090581055701</v>
       </c>
       <c r="AG49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AH49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>57.225433283399752</v>
       </c>
       <c r="AI49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8.5484015741282242</v>
       </c>
-    </row>
-    <row r="50" spans="7:38" x14ac:dyDescent="0.3">
+      <c r="AK49">
+        <v>-0.38240000000000002</v>
+      </c>
+      <c r="AL49">
+        <v>0.51</v>
+      </c>
+      <c r="AM49">
+        <v>-0.99880000000000002</v>
+      </c>
+      <c r="AN49">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G50" s="16" t="s">
         <v>114</v>
       </c>
@@ -4921,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G51" s="16" t="s">
         <v>116</v>
       </c>
@@ -4966,7 +5150,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G52" s="16" t="s">
         <v>67</v>
       </c>
@@ -4984,35 +5168,35 @@
         <v>0</v>
       </c>
       <c r="AD52">
-        <f t="shared" ref="AD52" si="6">$AC$39-AC52</f>
+        <f t="shared" ref="AD52" si="12">$AC$39-AC52</f>
         <v>2439.4</v>
       </c>
       <c r="AE52">
-        <f t="shared" ref="AE52:AJ52" si="7">AE35</f>
+        <f t="shared" ref="AE52:AJ52" si="13">AE35</f>
         <v>0</v>
       </c>
       <c r="AF52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>3100</v>
       </c>
       <c r="AG52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>398.15</v>
       </c>
       <c r="AH52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>120</v>
       </c>
       <c r="AI52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
       <c r="AJ52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>9.9999999999999992E+22</v>
       </c>
     </row>
-    <row r="53" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G53" s="16" t="s">
         <v>122</v>
       </c>
@@ -5027,35 +5211,35 @@
         <v>89</v>
       </c>
       <c r="AC53">
-        <f t="shared" ref="AC53:AC56" si="8">AC36</f>
+        <f t="shared" ref="AC53:AC56" si="14">AC36</f>
         <v>112.45399999999999</v>
       </c>
       <c r="AE53">
-        <f t="shared" ref="AE53:AJ56" si="9">AE36</f>
+        <f t="shared" ref="AE53:AJ56" si="15">AE36</f>
         <v>1.3422000000000001</v>
       </c>
       <c r="AF53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3307.6</v>
       </c>
       <c r="AG53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1099.75</v>
       </c>
       <c r="AH53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>129.89999999999998</v>
       </c>
       <c r="AI53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>65</v>
       </c>
       <c r="AJ53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>100000000000</v>
       </c>
     </row>
-    <row r="54" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:40" x14ac:dyDescent="0.3">
       <c r="G54" s="16" t="s">
         <v>119</v>
       </c>
@@ -5070,97 +5254,97 @@
         <v>85</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1326.0509999999999</v>
       </c>
       <c r="AE54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4.3647</v>
       </c>
       <c r="AF54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>7019</v>
       </c>
       <c r="AG54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1800</v>
       </c>
       <c r="AH54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>85.9</v>
       </c>
       <c r="AI54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ54">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="7:38" x14ac:dyDescent="0.3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="7:40" x14ac:dyDescent="0.3">
       <c r="AB55" t="s">
         <v>55</v>
       </c>
       <c r="AC55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2011.5958000000001</v>
       </c>
       <c r="AE55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>21.886399999999998</v>
       </c>
       <c r="AF55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>7225</v>
       </c>
       <c r="AG55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2450</v>
       </c>
       <c r="AH55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>127</v>
       </c>
       <c r="AI55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="AJ55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1E+20</v>
       </c>
     </row>
-    <row r="56" spans="7:38" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:40" x14ac:dyDescent="0.3">
       <c r="AB56" t="s">
         <v>180</v>
       </c>
       <c r="AC56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2439.4</v>
       </c>
       <c r="AE56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>35.418999999999997</v>
       </c>
       <c r="AF56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="AG56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2450</v>
       </c>
       <c r="AH56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="AI56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="AJ56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
     </row>
@@ -11882,28 +12066,28 @@
       <c r="C90"/>
       <c r="E90"/>
       <c r="F90"/>
-      <c r="G90" s="19" t="s">
+      <c r="G90" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
-      <c r="J90" s="19"/>
-      <c r="K90" s="19"/>
-      <c r="L90" s="19"/>
-      <c r="M90" s="19" t="s">
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="N90" s="19"/>
-      <c r="O90" s="19"/>
-      <c r="P90" s="19"/>
-      <c r="Q90" s="19"/>
-      <c r="R90" s="19"/>
-      <c r="S90" s="19" t="s">
+      <c r="N90" s="20"/>
+      <c r="O90" s="20"/>
+      <c r="P90" s="20"/>
+      <c r="Q90" s="20"/>
+      <c r="R90" s="20"/>
+      <c r="S90" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="T90" s="19"/>
-      <c r="U90" s="19"/>
-      <c r="V90" s="19"/>
+      <c r="T90" s="20"/>
+      <c r="U90" s="20"/>
+      <c r="V90" s="20"/>
       <c r="AD90"/>
       <c r="AG90"/>
     </row>

</xml_diff>